<commit_message>
add some debug file
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -7,31 +7,32 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="825"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="11" r:id="rId1"/>
-    <sheet name="article" sheetId="8" r:id="rId2"/>
-    <sheet name="top" sheetId="12" r:id="rId3"/>
-    <sheet name="success" sheetId="15" r:id="rId4"/>
-    <sheet name="error" sheetId="16" r:id="rId5"/>
-    <sheet name="layers" sheetId="7" r:id="rId6"/>
-    <sheet name="form" sheetId="2" r:id="rId7"/>
-    <sheet name="ui" sheetId="3" r:id="rId8"/>
-    <sheet name="feedback" sheetId="4" r:id="rId9"/>
-    <sheet name="nav" sheetId="5" r:id="rId10"/>
-    <sheet name="search" sheetId="6" r:id="rId11"/>
+    <sheet name="index" sheetId="17" r:id="rId1"/>
+    <sheet name="login" sheetId="11" r:id="rId2"/>
+    <sheet name="article" sheetId="8" r:id="rId3"/>
+    <sheet name="top" sheetId="12" r:id="rId4"/>
+    <sheet name="success" sheetId="15" r:id="rId5"/>
+    <sheet name="error" sheetId="16" r:id="rId6"/>
+    <sheet name="layers" sheetId="7" r:id="rId7"/>
+    <sheet name="form" sheetId="2" r:id="rId8"/>
+    <sheet name="ui" sheetId="3" r:id="rId9"/>
+    <sheet name="feedback" sheetId="4" r:id="rId10"/>
+    <sheet name="nav" sheetId="5" r:id="rId11"/>
+    <sheet name="search" sheetId="6" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">article!$A$1:$H$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">error!$A$1:$H$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">login!$A$1:$H$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">success!$A$1:$H$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">top!$A$1:$H$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">article!$A$1:$H$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">error!$A$1:$H$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">login!$A$1:$H$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">success!$A$1:$H$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">top!$A$1:$H$36</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>ページタイトル</t>
     <phoneticPr fontId="1"/>
@@ -281,12 +282,16 @@
     <t>内容１</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>Copyright © 2008-2016 KPF</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,7 +348,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,8 +367,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -488,6 +499,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -495,7 +586,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -519,6 +610,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -645,26 +755,50 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -690,29 +824,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2366,28 +2485,1200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AB43"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AM14" sqref="AM14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="1.375" customWidth="1"/>
+    <col min="24" max="24" width="2.625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="15"/>
+    </row>
+    <row r="3" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="16"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="17"/>
+    </row>
+    <row r="4" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="16"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="17"/>
+    </row>
+    <row r="5" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="16"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="17"/>
+    </row>
+    <row r="6" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="16"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="17"/>
+    </row>
+    <row r="7" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="16"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="17"/>
+    </row>
+    <row r="8" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="17"/>
+    </row>
+    <row r="9" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="16"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="16"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="17"/>
+    </row>
+    <row r="11" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="16"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="17"/>
+    </row>
+    <row r="12" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="16"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="17"/>
+    </row>
+    <row r="13" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="16"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="17"/>
+    </row>
+    <row r="14" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="16"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="17"/>
+    </row>
+    <row r="15" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="16"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="17"/>
+    </row>
+    <row r="16" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="16"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="17"/>
+    </row>
+    <row r="17" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="16"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="17"/>
+    </row>
+    <row r="18" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="16"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="17"/>
+    </row>
+    <row r="19" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="16"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="17"/>
+    </row>
+    <row r="20" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="16"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="17"/>
+    </row>
+    <row r="21" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="16"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="17"/>
+    </row>
+    <row r="22" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="16"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="17"/>
+    </row>
+    <row r="23" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="16"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="17"/>
+    </row>
+    <row r="24" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="16"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="17"/>
+    </row>
+    <row r="25" spans="2:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="16"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="17"/>
+    </row>
+    <row r="26" spans="2:28" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="84"/>
+      <c r="J26" s="84"/>
+      <c r="K26" s="84"/>
+      <c r="L26" s="84"/>
+      <c r="M26" s="84"/>
+      <c r="N26" s="84"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
+      <c r="S26" s="84"/>
+      <c r="T26" s="84"/>
+      <c r="U26" s="84"/>
+      <c r="V26" s="84"/>
+      <c r="W26" s="84"/>
+      <c r="X26" s="85"/>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11"/>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="11"/>
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="11"/>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="11"/>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="11"/>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="11"/>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="11"/>
+      <c r="AA42" s="11"/>
+      <c r="AB42" s="11"/>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.15">
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
+      <c r="AA43" s="11"/>
+      <c r="AB43" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B26:X26"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2396,7 +3687,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -2404,7 +3695,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -2412,7 +3703,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="13.5" customHeight="1">
+    <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -2420,7 +3711,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2428,7 +3719,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -2436,20 +3727,20 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B8" s="9"/>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="9"/>
       <c r="I8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -2457,34 +3748,34 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B10" s="9"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B11" s="8"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="8"/>
       <c r="I11" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B12" s="6"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -2492,7 +3783,7 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -2500,7 +3791,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -2508,20 +3799,20 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B16" s="9"/>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="9"/>
       <c r="I16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -2529,34 +3820,34 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B18" s="9"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B19" s="9"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="9"/>
       <c r="I19" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B20" s="8"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2564,7 +3855,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2572,7 +3863,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2580,36 +3871,36 @@
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="27" spans="2:9">
-      <c r="B27" s="11" t="s">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="2:9">
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="23"/>
       <c r="I28" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="19"/>
-    </row>
-    <row r="30" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="26"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -2617,7 +3908,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -2625,7 +3916,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2633,17 +3924,17 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="14.25">
-      <c r="A36" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
+    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A36" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="2" t="s">
         <v>2</v>
       </c>
@@ -2665,39 +3956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
@@ -2705,22 +3964,22 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2729,7 +3988,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2737,60 +3996,60 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13.5" customHeight="1">
-      <c r="B5" s="36" t="s">
+    <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="45"/>
       <c r="I5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="B6" s="39"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="40"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="B7" s="39"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="40"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="B8" s="39"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="40"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="B9" s="39"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="40"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="B10" s="41"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="43"/>
-    </row>
-    <row r="11" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B6" s="46"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="47"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B7" s="46"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="47"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B8" s="46"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="47"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B9" s="46"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="47"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2798,7 +4057,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
@@ -2811,7 +4070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2819,60 +4078,60 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:13">
-      <c r="B14" s="36" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B14" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="45"/>
       <c r="I14" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="B15" s="39"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="40"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="B16" s="39"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="40"/>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="39"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="40"/>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" s="39"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="40"/>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" s="41"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
-    </row>
-    <row r="20" spans="2:9">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B15" s="46"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="47"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B16" s="46"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="47"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B17" s="46"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="47"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B18" s="46"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="47"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2880,7 +4139,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -2888,7 +4147,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
@@ -2901,7 +4160,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2909,60 +4168,60 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:9">
-      <c r="B24" s="36" t="s">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B24" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="45"/>
       <c r="I24" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
-      <c r="B25" s="39"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="40"/>
-    </row>
-    <row r="26" spans="2:9">
-      <c r="B26" s="39"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="40"/>
-    </row>
-    <row r="27" spans="2:9">
-      <c r="B27" s="39"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="40"/>
-    </row>
-    <row r="28" spans="2:9">
-      <c r="B28" s="39"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="40"/>
-    </row>
-    <row r="29" spans="2:9">
-      <c r="B29" s="41"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="43"/>
-    </row>
-    <row r="30" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B25" s="46"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="47"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B26" s="46"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="47"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B27" s="46"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="47"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B28" s="46"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="47"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="50"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2970,7 +4229,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2978,7 +4237,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2986,17 +4245,17 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="14.25">
-      <c r="A36" s="23" t="s">
+    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A36" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="2" t="s">
         <v>2</v>
       </c>
@@ -3016,30 +4275,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="A14" sqref="A14:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3048,7 +4307,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -3059,7 +4318,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -3067,352 +4326,352 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="49"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56"/>
       <c r="I6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="50"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="52"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="44" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="59"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A8" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="53"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="56"/>
       <c r="I9" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="50"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="52"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="44" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A10" s="57"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="59"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A11" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="46"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="47"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="53"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A12" s="54"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="50"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="52"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="44" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A13" s="57"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="59"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A14" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="47"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="53"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A15" s="54"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="56"/>
       <c r="I15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="52"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="44" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A16" s="57"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="59"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="47"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="49"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="54"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="56"/>
       <c r="I18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="50"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="44" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="57"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="59"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="46"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="47"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="53"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="54"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="56"/>
       <c r="I21" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="50"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="52"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="44" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="57"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="59"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="46"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="47"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="49"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="54"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="56"/>
       <c r="I24" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="52"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="44" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="57"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="59"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="46"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="47"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="49"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="53"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="56"/>
       <c r="I27" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="50"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="52"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="44" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="57"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="59"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="46"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="47"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="53"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" s="54"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56"/>
       <c r="I30" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="50"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="52"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="44"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="46"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="47"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="49"/>
-    </row>
-    <row r="36" spans="1:9" ht="14.25">
-      <c r="A36" s="23" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" s="57"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="59"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="51"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="53"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33" s="54"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="56"/>
+    </row>
+    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A36" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="2" t="s">
         <v>2</v>
       </c>
@@ -3439,7 +4698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
@@ -3447,22 +4706,22 @@
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3471,7 +4730,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -3481,7 +4740,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -3491,7 +4750,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="13.5" customHeight="1">
+    <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -3501,24 +4760,24 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -3526,37 +4785,37 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -3566,22 +4825,22 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
       <c r="H12" s="10"/>
       <c r="I12" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -3591,7 +4850,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -3601,72 +4860,72 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="69"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
       <c r="H15" s="10"/>
       <c r="I15" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="10"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="72"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="71"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="10"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="72"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="71"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="10"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="72"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="71"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="75"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="74"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -3676,7 +4935,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -3686,7 +4945,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -3696,7 +4955,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -3706,42 +4965,42 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="10"/>
       <c r="I26" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -3751,7 +5010,7 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -3761,7 +5020,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -3771,7 +5030,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -3781,7 +5040,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -3791,7 +5050,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -3801,17 +5060,17 @@
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="14.25">
-      <c r="A36" s="23" t="s">
+    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A36" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="2" t="s">
         <v>2</v>
       </c>
@@ -3832,7 +5091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
@@ -3840,22 +5099,22 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3864,7 +5123,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -3874,7 +5133,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -3884,7 +5143,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="13.5" customHeight="1">
+    <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -3894,34 +5153,34 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -3929,27 +5188,27 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -3959,22 +5218,22 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
       <c r="H12" s="10"/>
       <c r="I12" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -3984,7 +5243,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -3994,72 +5253,72 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="61"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="76"/>
       <c r="H15" s="10"/>
       <c r="I15" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="64"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="10"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="64"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="10"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="64"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="10"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="64"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="67"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="82"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -4069,7 +5328,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -4079,7 +5338,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -4089,7 +5348,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -4099,42 +5358,42 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="10"/>
       <c r="I26" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -4144,7 +5403,7 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -4154,7 +5413,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -4164,7 +5423,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -4174,7 +5433,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -4184,7 +5443,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -4194,17 +5453,17 @@
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="14.25">
-      <c r="A36" s="23" t="s">
+    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A36" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="2" t="s">
         <v>2</v>
       </c>
@@ -4225,7 +5484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4233,7 +5492,7 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4241,7 +5500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4249,7 +5508,7 @@
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4258,7 +5517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4266,23 +5525,7 @@
       <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add simple input control
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Copyright © 2008-2016 KPF</t>
     <phoneticPr fontId="1"/>
@@ -317,31 +317,38 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w'w</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>阿德</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>sss</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>submit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>submit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>発信</t>
+    <rPh sb="0" eb="2">
+      <t>ハッシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://api.9jialu.com/profile/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>file</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ファイル</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -352,7 +359,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +550,14 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -721,13 +736,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1004,56 +1020,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
@@ -1081,8 +1052,56 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="ハイパーリンク" xfId="2" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1"/>
   </cellStyles>
@@ -1390,7 +1409,7 @@
   <dimension ref="A1:AL42"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AK20" sqref="AK20"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3826,8 +3845,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AN42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AN16" sqref="AN16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3857,7 +3876,7 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="119"/>
+      <c r="N1" s="104"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -3870,31 +3889,25 @@
       <c r="Y1" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="114"/>
-      <c r="AA1" s="114"/>
-      <c r="AB1" s="114"/>
+      <c r="Z1" s="123"/>
+      <c r="AA1" s="99"/>
+      <c r="AB1" s="99"/>
       <c r="AC1" s="64"/>
       <c r="AN1" s="87"/>
     </row>
     <row r="2" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
-      <c r="B2" s="109" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="103" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
       <c r="I2" s="13"/>
-      <c r="J2" s="110" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
       <c r="M2" s="14"/>
       <c r="N2" s="15"/>
       <c r="O2" s="14"/>
@@ -3909,27 +3922,29 @@
       <c r="Y2" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="Z2" s="112"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
+      <c r="Z2" s="124" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
       <c r="AC2" s="93"/>
       <c r="AN2" s="87"/>
     </row>
     <row r="3" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="120"/>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="122"/>
+      <c r="A3" s="105"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="107"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -3942,9 +3957,11 @@
       <c r="Y3" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="115"/>
-      <c r="AA3" s="116"/>
-      <c r="AB3" s="116"/>
+      <c r="Z3" s="100" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA3" s="101"/>
+      <c r="AB3" s="101"/>
       <c r="AC3" s="38"/>
       <c r="AN3" s="87"/>
     </row>
@@ -3984,7 +4001,7 @@
       <c r="AB4" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="AC4" s="113" t="s">
+      <c r="AC4" s="98" t="s">
         <v>38</v>
       </c>
       <c r="AN4" s="87"/>
@@ -3994,12 +4011,12 @@
       <c r="B5" s="75"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107" t="str">
-        <f>Z4</f>
-        <v>name</v>
-      </c>
-      <c r="G5" s="108"/>
+      <c r="E5" s="94" t="str">
+        <f>Y6</f>
+        <v>file</v>
+      </c>
+      <c r="F5" s="94"/>
+      <c r="G5" s="95"/>
       <c r="H5" s="90"/>
       <c r="I5" s="90"/>
       <c r="J5" s="90"/>
@@ -4016,12 +4033,18 @@
       <c r="U5" s="74"/>
       <c r="V5" s="74"/>
       <c r="W5" s="21"/>
-      <c r="Y5" s="92"/>
-      <c r="Z5" s="92"/>
+      <c r="Y5" s="92" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" s="92" t="s">
+        <v>42</v>
+      </c>
       <c r="AA5" s="88" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB5" s="92"/>
+        <v>41</v>
+      </c>
+      <c r="AB5" s="92" t="s">
+        <v>43</v>
+      </c>
       <c r="AC5" s="61"/>
       <c r="AE5" s="87"/>
       <c r="AF5" s="87"/>
@@ -4054,10 +4077,18 @@
       <c r="U6" s="74"/>
       <c r="V6" s="74"/>
       <c r="W6" s="21"/>
-      <c r="Y6" s="92"/>
-      <c r="Z6" s="92"/>
-      <c r="AA6" s="112"/>
-      <c r="AB6" s="92"/>
+      <c r="Y6" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z6" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA6" s="97" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB6" s="92" t="s">
+        <v>47</v>
+      </c>
       <c r="AC6" s="61"/>
       <c r="AE6" s="87"/>
       <c r="AF6" s="87"/>
@@ -4067,11 +4098,9 @@
       <c r="AN6" s="87"/>
     </row>
     <row r="7" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="A7" s="6"/>
       <c r="B7" s="78"/>
-      <c r="C7" s="117"/>
+      <c r="C7" s="102"/>
       <c r="D7" s="89"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
@@ -4094,7 +4123,7 @@
       <c r="W7" s="21"/>
       <c r="Y7" s="92"/>
       <c r="Z7" s="92"/>
-      <c r="AA7" s="112"/>
+      <c r="AA7" s="97"/>
       <c r="AB7" s="92"/>
       <c r="AC7" s="61"/>
       <c r="AE7" s="87"/>
@@ -4107,26 +4136,22 @@
     <row r="8" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6"/>
       <c r="B8" s="79"/>
-      <c r="C8" s="117"/>
+      <c r="C8" s="102"/>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
-      <c r="F8" s="28" t="str">
-        <f>Y4</f>
-        <v>id</v>
-      </c>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
-      <c r="J8" s="94" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="95"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="95"/>
-      <c r="N8" s="95"/>
-      <c r="O8" s="95"/>
-      <c r="P8" s="95"/>
-      <c r="Q8" s="96"/>
+      <c r="J8" s="114" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="115"/>
+      <c r="L8" s="115"/>
+      <c r="M8" s="115"/>
+      <c r="N8" s="115"/>
+      <c r="O8" s="115"/>
+      <c r="P8" s="115"/>
+      <c r="Q8" s="116"/>
       <c r="R8" s="28"/>
       <c r="S8" s="28"/>
       <c r="T8" s="28"/>
@@ -4135,7 +4160,7 @@
       <c r="W8" s="26"/>
       <c r="Y8" s="92"/>
       <c r="Z8" s="92"/>
-      <c r="AA8" s="112"/>
+      <c r="AA8" s="97"/>
       <c r="AB8" s="92"/>
       <c r="AC8" s="61"/>
       <c r="AE8" s="87"/>
@@ -4147,21 +4172,21 @@
     <row r="9" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6"/>
       <c r="B9" s="28"/>
-      <c r="C9" s="117"/>
+      <c r="C9" s="102"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="97"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="98"/>
-      <c r="P9" s="98"/>
-      <c r="Q9" s="99"/>
+      <c r="J9" s="117"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="118"/>
+      <c r="N9" s="118"/>
+      <c r="O9" s="118"/>
+      <c r="P9" s="118"/>
+      <c r="Q9" s="119"/>
       <c r="R9" s="28"/>
       <c r="S9" s="28"/>
       <c r="T9" s="28"/>
@@ -4170,7 +4195,7 @@
       <c r="W9" s="26"/>
       <c r="Y9" s="92"/>
       <c r="Z9" s="92"/>
-      <c r="AA9" s="112"/>
+      <c r="AA9" s="97"/>
       <c r="AB9" s="92"/>
       <c r="AC9" s="61"/>
       <c r="AE9" s="87"/>
@@ -4182,21 +4207,21 @@
     <row r="10" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6"/>
       <c r="B10" s="28"/>
-      <c r="C10" s="117"/>
+      <c r="C10" s="102"/>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
-      <c r="N10" s="98"/>
-      <c r="O10" s="98"/>
-      <c r="P10" s="98"/>
-      <c r="Q10" s="99"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="118"/>
+      <c r="M10" s="118"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="118"/>
+      <c r="P10" s="118"/>
+      <c r="Q10" s="119"/>
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
@@ -4205,7 +4230,7 @@
       <c r="W10" s="26"/>
       <c r="Y10" s="92"/>
       <c r="Z10" s="92"/>
-      <c r="AA10" s="112"/>
+      <c r="AA10" s="97"/>
       <c r="AB10" s="92"/>
       <c r="AC10" s="61"/>
       <c r="AE10" s="87"/>
@@ -4217,21 +4242,21 @@
     <row r="11" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6"/>
       <c r="B11" s="28"/>
-      <c r="C11" s="117"/>
+      <c r="C11" s="102"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="97"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="98"/>
-      <c r="O11" s="98"/>
-      <c r="P11" s="98"/>
-      <c r="Q11" s="99"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="118"/>
+      <c r="N11" s="118"/>
+      <c r="O11" s="118"/>
+      <c r="P11" s="118"/>
+      <c r="Q11" s="119"/>
       <c r="R11" s="28"/>
       <c r="S11" s="28"/>
       <c r="T11" s="28"/>
@@ -4240,7 +4265,7 @@
       <c r="W11" s="26"/>
       <c r="Y11" s="92"/>
       <c r="Z11" s="92"/>
-      <c r="AA11" s="112"/>
+      <c r="AA11" s="97"/>
       <c r="AB11" s="92"/>
       <c r="AC11" s="61"/>
       <c r="AE11" s="87"/>
@@ -4252,21 +4277,21 @@
     <row r="12" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6"/>
       <c r="B12" s="28"/>
-      <c r="C12" s="117"/>
+      <c r="C12" s="102"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="101"/>
-      <c r="M12" s="101"/>
-      <c r="N12" s="101"/>
-      <c r="O12" s="101"/>
-      <c r="P12" s="101"/>
-      <c r="Q12" s="102"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="121"/>
+      <c r="L12" s="121"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="121"/>
+      <c r="P12" s="121"/>
+      <c r="Q12" s="122"/>
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
       <c r="T12" s="28"/>
@@ -4277,7 +4302,7 @@
     <row r="13" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6"/>
       <c r="B13" s="28"/>
-      <c r="C13" s="117"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
@@ -4296,32 +4321,32 @@
       <c r="S13" s="28"/>
       <c r="T13" s="28"/>
       <c r="U13" s="28"/>
-      <c r="V13" s="17"/>
+      <c r="V13" s="24"/>
       <c r="W13" s="26"/>
     </row>
     <row r="14" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6"/>
       <c r="B14" s="28"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="118"/>
-      <c r="K14" s="118"/>
-      <c r="L14" s="118"/>
-      <c r="M14" s="118"/>
-      <c r="N14" s="118"/>
-      <c r="O14" s="118"/>
-      <c r="P14" s="118"/>
-      <c r="Q14" s="118"/>
-      <c r="R14" s="118"/>
-      <c r="S14" s="118"/>
-      <c r="T14" s="118"/>
-      <c r="U14" s="118"/>
-      <c r="V14" s="107"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="103"/>
+      <c r="K14" s="103"/>
+      <c r="L14" s="103"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="103"/>
+      <c r="O14" s="103"/>
+      <c r="P14" s="103"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="103"/>
+      <c r="S14" s="103"/>
+      <c r="T14" s="103"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="31"/>
       <c r="W14" s="26"/>
     </row>
     <row r="15" spans="1:40" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -4377,7 +4402,10 @@
     <row r="17" spans="1:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6"/>
       <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="C17" s="28" t="str">
+        <f>Y5</f>
+        <v>submit</v>
+      </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
@@ -4450,9 +4478,7 @@
       <c r="W19" s="7"/>
     </row>
     <row r="20" spans="1:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="A20" s="8"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -4577,31 +4603,31 @@
       <c r="W24" s="7"/>
     </row>
     <row r="25" spans="1:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="105" t="s">
+      <c r="A25" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="104"/>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="104"/>
-      <c r="G25" s="104"/>
-      <c r="H25" s="104"/>
-      <c r="I25" s="104"/>
-      <c r="J25" s="104"/>
-      <c r="K25" s="104"/>
-      <c r="L25" s="104"/>
-      <c r="M25" s="104"/>
-      <c r="N25" s="104"/>
-      <c r="O25" s="104"/>
-      <c r="P25" s="104"/>
-      <c r="Q25" s="104"/>
-      <c r="R25" s="104"/>
-      <c r="S25" s="104"/>
-      <c r="T25" s="104"/>
-      <c r="U25" s="104"/>
-      <c r="V25" s="104"/>
-      <c r="W25" s="106"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="109"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="109"/>
+      <c r="J25" s="109"/>
+      <c r="K25" s="109"/>
+      <c r="L25" s="109"/>
+      <c r="M25" s="109"/>
+      <c r="N25" s="109"/>
+      <c r="O25" s="109"/>
+      <c r="P25" s="109"/>
+      <c r="Q25" s="109"/>
+      <c r="R25" s="109"/>
+      <c r="S25" s="109"/>
+      <c r="T25" s="109"/>
+      <c r="U25" s="109"/>
+      <c r="V25" s="109"/>
+      <c r="W25" s="110"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A26" s="13"/>
@@ -5021,8 +5047,11 @@
     <mergeCell ref="J8:Q12"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="Z2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -5044,7 +5073,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add css create logic
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="825" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="825" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="home" sheetId="22" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="sale" sheetId="27" r:id="rId4"/>
     <sheet name="map" sheetId="24" r:id="rId5"/>
     <sheet name="_data" sheetId="21" r:id="rId6"/>
+    <sheet name="_css" sheetId="28" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">home!$A$1:$T$35</definedName>
@@ -603,7 +604,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="417">
   <si>
     <t>action</t>
     <phoneticPr fontId="5"/>
@@ -848,14 +849,6 @@
   <si>
     <t>onclick</t>
     <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>redirect('home')</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>redirect('profile')</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>XXXXXXX</t>
@@ -949,14 +942,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>redirect('project')</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>redirect('profile')</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>MyProject</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -973,14 +958,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>redirect('map')</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>redirect('sale')</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>edit</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -1033,6 +1010,999 @@
   <si>
     <t>{ user.displayName }</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>{redirect('home')}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{redirect('profile')}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{edit}</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>{redirect('project')}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{redirect('sale')}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{redirect('map')}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>@CHARSET "UTF-8";</t>
+  </si>
+  <si>
+    <t>font-family: 'メイリオ', Meiryo, 'ＭＳ Ｐゴシック', sans-serif;</t>
+  </si>
+  <si>
+    <t>height: 1rem;</t>
+  </si>
+  <si>
+    <t>position: absolute;</t>
+  </si>
+  <si>
+    <t>width: 2rem;</t>
+  </si>
+  <si>
+    <t>width: 3rem;</t>
+  </si>
+  <si>
+    <t>width: 5rem;</t>
+  </si>
+  <si>
+    <t>width: 6rem;</t>
+  </si>
+  <si>
+    <t>width: 7rem;</t>
+  </si>
+  <si>
+    <t>width: 8rem;</t>
+  </si>
+  <si>
+    <t>width: 9rem;</t>
+  </si>
+  <si>
+    <t>width: 10rem;</t>
+  </si>
+  <si>
+    <t>width: 11rem;</t>
+  </si>
+  <si>
+    <t>width: 12rem;</t>
+  </si>
+  <si>
+    <t>width: 13rem;</t>
+  </si>
+  <si>
+    <t>width: 14rem;</t>
+  </si>
+  <si>
+    <t>width: 15rem;</t>
+  </si>
+  <si>
+    <t>width: 16rem;</t>
+  </si>
+  <si>
+    <t>width: 17rem;</t>
+  </si>
+  <si>
+    <t>width: 18rem;</t>
+  </si>
+  <si>
+    <t>width: 19rem;</t>
+  </si>
+  <si>
+    <t>width: 20rem;</t>
+  </si>
+  <si>
+    <t>width: 21rem;</t>
+  </si>
+  <si>
+    <t>width: 22rem;</t>
+  </si>
+  <si>
+    <t>width: 23rem;</t>
+  </si>
+  <si>
+    <t>height: 2rem;</t>
+  </si>
+  <si>
+    <t>height: 3rem;</t>
+  </si>
+  <si>
+    <t>height: 4rem;</t>
+  </si>
+  <si>
+    <t>height: 6rem;</t>
+  </si>
+  <si>
+    <t>height: 7rem;</t>
+  </si>
+  <si>
+    <t>height: 8rem;</t>
+  </si>
+  <si>
+    <t>height: 9rem;</t>
+  </si>
+  <si>
+    <t>height: 10rem;</t>
+  </si>
+  <si>
+    <t>height: 11rem;</t>
+  </si>
+  <si>
+    <t>height: 12rem;</t>
+  </si>
+  <si>
+    <t>height: 13rem;</t>
+  </si>
+  <si>
+    <t>height: 14rem;</t>
+  </si>
+  <si>
+    <t>height: 15rem;</t>
+  </si>
+  <si>
+    <t>display: -webkit-flex;</t>
+  </si>
+  <si>
+    <t>-webkit-justify-content: flex-start;</t>
+  </si>
+  <si>
+    <t>justify-content: flex-start;</t>
+  </si>
+  <si>
+    <t>display: flex;</t>
+  </si>
+  <si>
+    <t>-webkit-justify-content: center;</t>
+  </si>
+  <si>
+    <t>justify-content: center;</t>
+  </si>
+  <si>
+    <t>-webkit-justify-content: flex-end;</t>
+  </si>
+  <si>
+    <t>justify-content: flex-end;</t>
+  </si>
+  <si>
+    <t>-webkit-align-items: flex-start;</t>
+  </si>
+  <si>
+    <t>-webkit-align-items: center;</t>
+  </si>
+  <si>
+    <t>align-items: center;</t>
+  </si>
+  <si>
+    <t>-webkit-align-items: flex-end;</t>
+  </si>
+  <si>
+    <t>align-items: flex-end;</t>
+  </si>
+  <si>
+    <t>z-index: 10;</t>
+  </si>
+  <si>
+    <t>border-top: 1px dashed #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-top: 1px solid #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-top: 3px double #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-bottom: 1px dotted #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-bottom: 1px dashed #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-bottom: 1px solid #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-bottom: 3px double #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-left: 1px dotted #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-left: 1px dashed #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-left: 1px solid #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-left: 3px double #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-right: 1px dotted #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-right: 1px dashed #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-right: 1px solid #5F6F7E;</t>
+  </si>
+  <si>
+    <t>border-right: 3px double #5F6F7E;</t>
+  </si>
+  <si>
+    <t>top: 0rem;</t>
+  </si>
+  <si>
+    <t>top: 1rem;</t>
+  </si>
+  <si>
+    <t>top: 3rem;</t>
+  </si>
+  <si>
+    <t>top: 4rem;</t>
+  </si>
+  <si>
+    <t>top: 5rem;</t>
+  </si>
+  <si>
+    <t>top: 6rem;</t>
+  </si>
+  <si>
+    <t>top: 7rem;</t>
+  </si>
+  <si>
+    <t>top: 8rem;</t>
+  </si>
+  <si>
+    <t>top: 9rem;</t>
+  </si>
+  <si>
+    <t>top: 10rem;</t>
+  </si>
+  <si>
+    <t>top: 11rem;</t>
+  </si>
+  <si>
+    <t>top: 12rem;</t>
+  </si>
+  <si>
+    <t>top: 13rem;</t>
+  </si>
+  <si>
+    <t>top: 14rem;</t>
+  </si>
+  <si>
+    <t>top: 15rem;</t>
+  </si>
+  <si>
+    <t>top: 16rem;</t>
+  </si>
+  <si>
+    <t>top: 17rem;</t>
+  </si>
+  <si>
+    <t>top: 18rem;</t>
+  </si>
+  <si>
+    <t>top: 19rem;</t>
+  </si>
+  <si>
+    <t>top: 20rem;</t>
+  </si>
+  <si>
+    <t>top: 21rem;</t>
+  </si>
+  <si>
+    <t>top: 22rem;</t>
+  </si>
+  <si>
+    <t>top: 23rem;</t>
+  </si>
+  <si>
+    <t>top: 24rem;</t>
+  </si>
+  <si>
+    <t>top: 25rem;</t>
+  </si>
+  <si>
+    <t>top: 26rem;</t>
+  </si>
+  <si>
+    <t>top: 27rem;</t>
+  </si>
+  <si>
+    <t>top: 28rem;</t>
+  </si>
+  <si>
+    <t>top: 29rem;</t>
+  </si>
+  <si>
+    <t>top: 30rem;</t>
+  </si>
+  <si>
+    <t>top: 31rem;</t>
+  </si>
+  <si>
+    <t>top: 32rem;</t>
+  </si>
+  <si>
+    <t>top: 33rem;</t>
+  </si>
+  <si>
+    <t>top: 34rem;</t>
+  </si>
+  <si>
+    <t>left: 0rem;</t>
+  </si>
+  <si>
+    <t>left: 1rem;</t>
+  </si>
+  <si>
+    <t>left: 2rem;</t>
+  </si>
+  <si>
+    <t>left: 3rem;</t>
+  </si>
+  <si>
+    <t>left: 4rem;</t>
+  </si>
+  <si>
+    <t>left: 5rem;</t>
+  </si>
+  <si>
+    <t>left: 6rem;</t>
+  </si>
+  <si>
+    <t>left: 7rem;</t>
+  </si>
+  <si>
+    <t>left: 8rem;</t>
+  </si>
+  <si>
+    <t>left: 9rem;</t>
+  </si>
+  <si>
+    <t>left: 10rem;</t>
+  </si>
+  <si>
+    <t>left: 11rem;</t>
+  </si>
+  <si>
+    <t>left: 12rem;</t>
+  </si>
+  <si>
+    <t>left: 13rem;</t>
+  </si>
+  <si>
+    <t>left: 14rem;</t>
+  </si>
+  <si>
+    <t>left: 15rem;</t>
+  </si>
+  <si>
+    <t>left: 16rem;</t>
+  </si>
+  <si>
+    <t>left: 17rem;</t>
+  </si>
+  <si>
+    <t>left: 18rem;</t>
+  </si>
+  <si>
+    <t>white-space: nowrap;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>line-height: 1rem;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>body</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pre</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>display: inline;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>input</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>height: 1rem;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>input:focus</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>outline: none !important;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>border: 2px solid #3a4782;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>box-shadow: 0 0 10px #719ECE;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>position: absolute;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>width: 1rem;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>z-index: -1;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.W1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>width: 1rem;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.W2</t>
+  </si>
+  <si>
+    <t>.W3</t>
+  </si>
+  <si>
+    <t>.W4</t>
+  </si>
+  <si>
+    <t>.W5</t>
+  </si>
+  <si>
+    <t>.W6</t>
+  </si>
+  <si>
+    <t>.W7</t>
+  </si>
+  <si>
+    <t>.W8</t>
+  </si>
+  <si>
+    <t>.W9</t>
+  </si>
+  <si>
+    <t>.W10</t>
+  </si>
+  <si>
+    <t>.W11</t>
+  </si>
+  <si>
+    <t>.W12</t>
+  </si>
+  <si>
+    <t>.W13</t>
+  </si>
+  <si>
+    <t>.W14</t>
+  </si>
+  <si>
+    <t>.W15</t>
+  </si>
+  <si>
+    <t>.W16</t>
+  </si>
+  <si>
+    <t>.W17</t>
+  </si>
+  <si>
+    <t>.W18</t>
+  </si>
+  <si>
+    <t>.W19</t>
+  </si>
+  <si>
+    <t>.W20</t>
+  </si>
+  <si>
+    <t>.W21</t>
+  </si>
+  <si>
+    <t>.W22</t>
+  </si>
+  <si>
+    <t>.W23</t>
+  </si>
+  <si>
+    <t>.H1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.H2</t>
+  </si>
+  <si>
+    <t>.H3</t>
+  </si>
+  <si>
+    <t>.H4</t>
+  </si>
+  <si>
+    <t>.H5</t>
+  </si>
+  <si>
+    <t>.H6</t>
+  </si>
+  <si>
+    <t>.H7</t>
+  </si>
+  <si>
+    <t>.H8</t>
+  </si>
+  <si>
+    <t>.H9</t>
+  </si>
+  <si>
+    <t>.H10</t>
+  </si>
+  <si>
+    <t>.H11</t>
+  </si>
+  <si>
+    <t>.H12</t>
+  </si>
+  <si>
+    <t>.H13</t>
+  </si>
+  <si>
+    <t>.H14</t>
+  </si>
+  <si>
+    <t>.H15</t>
+  </si>
+  <si>
+    <t>.H16</t>
+  </si>
+  <si>
+    <t>height: 16rem;</t>
+  </si>
+  <si>
+    <t>.H17</t>
+  </si>
+  <si>
+    <t>height: 17rem;</t>
+  </si>
+  <si>
+    <t>.H18</t>
+  </si>
+  <si>
+    <t>height: 18rem;</t>
+  </si>
+  <si>
+    <t>.H19</t>
+  </si>
+  <si>
+    <t>height: 19rem;</t>
+  </si>
+  <si>
+    <t>.H20</t>
+  </si>
+  <si>
+    <t>height: 20rem;</t>
+  </si>
+  <si>
+    <t>.H21</t>
+  </si>
+  <si>
+    <t>height: 21rem;</t>
+  </si>
+  <si>
+    <t>.H22</t>
+  </si>
+  <si>
+    <t>height: 22rem;</t>
+  </si>
+  <si>
+    <t>.H23</t>
+  </si>
+  <si>
+    <t>height: 23rem;</t>
+  </si>
+  <si>
+    <t>.H24</t>
+  </si>
+  <si>
+    <t>height: 24rem;</t>
+  </si>
+  <si>
+    <t>.H25</t>
+  </si>
+  <si>
+    <t>height: 25rem;</t>
+  </si>
+  <si>
+    <t>.H26</t>
+  </si>
+  <si>
+    <t>height: 26rem;</t>
+  </si>
+  <si>
+    <t>.H27</t>
+  </si>
+  <si>
+    <t>height: 27rem;</t>
+  </si>
+  <si>
+    <t>.H28</t>
+  </si>
+  <si>
+    <t>height: 28rem;</t>
+  </si>
+  <si>
+    <t>.H29</t>
+  </si>
+  <si>
+    <t>height: 29rem;</t>
+  </si>
+  <si>
+    <t>.H30</t>
+  </si>
+  <si>
+    <t>height: 30rem;</t>
+  </si>
+  <si>
+    <t>.H31</t>
+  </si>
+  <si>
+    <t>height: 31rem;</t>
+  </si>
+  <si>
+    <t>.H32</t>
+  </si>
+  <si>
+    <t>height: 32rem;</t>
+  </si>
+  <si>
+    <t>.H33</t>
+  </si>
+  <si>
+    <t>height: 33rem;</t>
+  </si>
+  <si>
+    <t>.H34</t>
+  </si>
+  <si>
+    <t>height: 34rem;</t>
+  </si>
+  <si>
+    <t>.TA1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.TA2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.TA3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.VA0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.VA1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.VA2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.I</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.IB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.BT1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.BT2</t>
+  </si>
+  <si>
+    <t>.BT3</t>
+  </si>
+  <si>
+    <t>.BT4</t>
+  </si>
+  <si>
+    <t>.BB1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.BB2</t>
+  </si>
+  <si>
+    <t>.BB3</t>
+  </si>
+  <si>
+    <t>.BB4</t>
+  </si>
+  <si>
+    <t>.BL1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.BL2</t>
+  </si>
+  <si>
+    <t>.BL3</t>
+  </si>
+  <si>
+    <t>.BL4</t>
+  </si>
+  <si>
+    <t>.BR1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.BR2</t>
+  </si>
+  <si>
+    <t>.BR3</t>
+  </si>
+  <si>
+    <t>.BR4</t>
+  </si>
+  <si>
+    <t>.R0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.R1</t>
+  </si>
+  <si>
+    <t>.R2</t>
+  </si>
+  <si>
+    <t>.R3</t>
+  </si>
+  <si>
+    <t>.R4</t>
+  </si>
+  <si>
+    <t>.R5</t>
+  </si>
+  <si>
+    <t>.R6</t>
+  </si>
+  <si>
+    <t>.R7</t>
+  </si>
+  <si>
+    <t>.R8</t>
+  </si>
+  <si>
+    <t>.R9</t>
+  </si>
+  <si>
+    <t>.R10</t>
+  </si>
+  <si>
+    <t>.R11</t>
+  </si>
+  <si>
+    <t>.R12</t>
+  </si>
+  <si>
+    <t>.R13</t>
+  </si>
+  <si>
+    <t>.R14</t>
+  </si>
+  <si>
+    <t>.R15</t>
+  </si>
+  <si>
+    <t>.R16</t>
+  </si>
+  <si>
+    <t>.R17</t>
+  </si>
+  <si>
+    <t>.R18</t>
+  </si>
+  <si>
+    <t>.R19</t>
+  </si>
+  <si>
+    <t>.R20</t>
+  </si>
+  <si>
+    <t>.R21</t>
+  </si>
+  <si>
+    <t>.R22</t>
+  </si>
+  <si>
+    <t>.R23</t>
+  </si>
+  <si>
+    <t>.R24</t>
+  </si>
+  <si>
+    <t>.R25</t>
+  </si>
+  <si>
+    <t>.R26</t>
+  </si>
+  <si>
+    <t>.R27</t>
+  </si>
+  <si>
+    <t>.R28</t>
+  </si>
+  <si>
+    <t>.R29</t>
+  </si>
+  <si>
+    <t>.R30</t>
+  </si>
+  <si>
+    <t>.R31</t>
+  </si>
+  <si>
+    <t>.R32</t>
+  </si>
+  <si>
+    <t>.R33</t>
+  </si>
+  <si>
+    <t>.R34</t>
+  </si>
+  <si>
+    <t>.C0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.C1</t>
+  </si>
+  <si>
+    <t>.C2</t>
+  </si>
+  <si>
+    <t>.C3</t>
+  </si>
+  <si>
+    <t>.C4</t>
+  </si>
+  <si>
+    <t>.C5</t>
+  </si>
+  <si>
+    <t>.C6</t>
+  </si>
+  <si>
+    <t>.C7</t>
+  </si>
+  <si>
+    <t>.C8</t>
+  </si>
+  <si>
+    <t>.C9</t>
+  </si>
+  <si>
+    <t>.C10</t>
+  </si>
+  <si>
+    <t>.C11</t>
+  </si>
+  <si>
+    <t>.C12</t>
+  </si>
+  <si>
+    <t>.C13</t>
+  </si>
+  <si>
+    <t>.C14</t>
+  </si>
+  <si>
+    <t>.C15</t>
+  </si>
+  <si>
+    <t>.C16</t>
+  </si>
+  <si>
+    <t>.C17</t>
+  </si>
+  <si>
+    <t>.C18</t>
+  </si>
+  <si>
+    <t>.C19</t>
+  </si>
+  <si>
+    <t>left: 18.9rem;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*body*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>width: 4rem;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*width*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>height: 5rem;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*height*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>align-items: flex-start;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*align*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>font-weight: bold;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*font*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>border-top: 1px dotted #5F6F7E;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*border*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>top: 2rem;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*cell top*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*cell left*/</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1892,111 +2862,19 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2053,6 +2931,42 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="25" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2088,6 +3002,62 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2399,7 +3369,7 @@
   <dimension ref="A1:AN52"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2570,7 +3540,7 @@
         <v>61</v>
       </c>
       <c r="AE4" s="29" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AN4" s="23"/>
     </row>
@@ -2599,16 +3569,16 @@
       <c r="V5" s="14"/>
       <c r="W5" s="14"/>
       <c r="Y5" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Z5" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA5" s="24" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB5" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AC5" s="11" t="s">
         <v>56</v>
@@ -2649,16 +3619,16 @@
       <c r="V6" s="14"/>
       <c r="W6" s="14"/>
       <c r="Y6" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Z6" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AA6" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB6" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
@@ -2703,7 +3673,7 @@
         <v>24</v>
       </c>
       <c r="AA7" s="28" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AB7" s="25"/>
       <c r="AC7" s="11"/>
@@ -2746,7 +3716,7 @@
         <v>26</v>
       </c>
       <c r="AA8" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB8" s="25"/>
       <c r="AC8" s="11"/>
@@ -2788,7 +3758,7 @@
         <v>27</v>
       </c>
       <c r="AA9" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="11"/>
@@ -2833,7 +3803,7 @@
         <v>28</v>
       </c>
       <c r="AA10" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="11"/>
@@ -2878,13 +3848,13 @@
         <v>32</v>
       </c>
       <c r="AB11" s="25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="AC11" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AD11" s="11" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="AE11" s="11"/>
       <c r="AF11" s="23"/>
@@ -2929,13 +3899,13 @@
         <v>32</v>
       </c>
       <c r="AB12" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AC12" s="11" t="s">
         <v>58</v>
       </c>
       <c r="AD12" s="11" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="AE12" s="11"/>
     </row>
@@ -2973,13 +3943,13 @@
         <v>32</v>
       </c>
       <c r="AB13" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AC13" s="11" t="s">
         <v>59</v>
       </c>
       <c r="AD13" s="11" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="AE13" s="11"/>
     </row>
@@ -3020,13 +3990,13 @@
         <v>32</v>
       </c>
       <c r="AB14" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AC14" s="11" t="s">
         <v>60</v>
       </c>
       <c r="AD14" s="11" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="AE14" s="11"/>
     </row>
@@ -3471,7 +4441,7 @@
       <c r="D32" s="73"/>
       <c r="E32" s="20"/>
       <c r="F32" s="67" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G32" s="67"/>
       <c r="H32" s="67"/>
@@ -3541,7 +4511,7 @@
     </row>
     <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="71"/>
@@ -4017,7 +4987,7 @@
   <dimension ref="A1:AE52"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Y34" sqref="Y34"/>
+      <selection activeCell="AQ18" sqref="AQ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4036,28 +5006,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
       <c r="U1" s="48"/>
       <c r="V1" s="48"/>
       <c r="W1" s="48"/>
@@ -4073,41 +5043,41 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="119" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="78" t="str">
+      <c r="B2" s="120"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="126" t="str">
         <f>Y12</f>
         <v>in6</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="74" t="s">
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="103" t="str">
+      <c r="I2" s="120"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="77" t="str">
         <f>Y17</f>
         <v>in11</v>
       </c>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="116" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="117"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="119" t="str">
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="92"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="103" t="str">
         <f>Y21</f>
         <v>in15</v>
       </c>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="121"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="105"/>
       <c r="U2" s="49"/>
       <c r="V2" s="49"/>
       <c r="W2" s="49"/>
@@ -4122,36 +5092,36 @@
       <c r="AC2" s="26"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="81" t="str">
+      <c r="B3" s="116"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="128" t="str">
         <f>Y13</f>
         <v>in7</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="87" t="s">
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="88"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="104" t="str">
+      <c r="I3" s="98"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="79" t="str">
         <f>Y18</f>
         <v>in12</v>
       </c>
-      <c r="L3" s="105"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="122"/>
-      <c r="R3" s="123"/>
-      <c r="S3" s="123"/>
-      <c r="T3" s="124"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="106"/>
+      <c r="R3" s="107"/>
+      <c r="S3" s="107"/>
+      <c r="T3" s="108"/>
       <c r="U3" s="49"/>
       <c r="V3" s="49"/>
       <c r="W3" s="49"/>
@@ -4166,36 +5136,36 @@
       <c r="AC3" s="8"/>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="81" t="str">
+      <c r="B4" s="116"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="128" t="str">
         <f>Y14</f>
         <v>in8</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="87" t="s">
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="88"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="125" t="str">
+      <c r="O4" s="98"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="109" t="str">
         <f>Y22</f>
         <v>in16</v>
       </c>
-      <c r="R4" s="126"/>
-      <c r="S4" s="126"/>
-      <c r="T4" s="127"/>
+      <c r="R4" s="110"/>
+      <c r="S4" s="110"/>
+      <c r="T4" s="111"/>
       <c r="U4" s="49"/>
       <c r="V4" s="49"/>
       <c r="W4" s="49"/>
@@ -4218,40 +5188,40 @@
         <v>61</v>
       </c>
       <c r="AE4" s="29" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="81" t="str">
+      <c r="B5" s="116"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="128" t="str">
         <f>Y15</f>
         <v>in9</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="93" t="s">
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="94"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="110" t="str">
+      <c r="I5" s="116"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="85" t="str">
         <f>Y19</f>
         <v>in13</v>
       </c>
-      <c r="L5" s="111"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="92"/>
-      <c r="Q5" s="122"/>
-      <c r="R5" s="123"/>
-      <c r="S5" s="123"/>
-      <c r="T5" s="124"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="107"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="108"/>
       <c r="U5" s="49"/>
       <c r="V5" s="49"/>
       <c r="W5" s="49"/>
@@ -4274,41 +5244,41 @@
       <c r="AE5" s="11"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="99" t="str">
+      <c r="B6" s="101"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="122" t="str">
         <f>Y16</f>
         <v>in10</v>
       </c>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="84" t="s">
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="113" t="str">
+      <c r="I6" s="101"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="88" t="str">
         <f>Y20</f>
         <v>in14</v>
       </c>
-      <c r="L6" s="114"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" s="85"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="128" t="str">
+      <c r="L6" s="89"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="101"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="112" t="str">
         <f>Y23</f>
         <v>in17</v>
       </c>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
-      <c r="T6" s="130"/>
+      <c r="R6" s="113"/>
+      <c r="S6" s="113"/>
+      <c r="T6" s="114"/>
       <c r="U6" s="50"/>
       <c r="V6" s="50"/>
       <c r="W6" s="50"/>
@@ -4329,9 +5299,9 @@
       <c r="AE6" s="11"/>
     </row>
     <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
+      <c r="A7" s="125"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -4449,19 +5419,19 @@
       <c r="B10" s="6"/>
       <c r="C10" s="57"/>
       <c r="D10" s="57"/>
-      <c r="E10" s="98" t="s">
+      <c r="E10" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="98" t="s">
+      <c r="F10" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="98" t="s">
+      <c r="G10" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="98" t="s">
+      <c r="H10" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="98" t="s">
+      <c r="I10" s="118" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="57"/>
@@ -4488,13 +5458,13 @@
         <v>32</v>
       </c>
       <c r="AB10" s="25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AC10" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AD10" s="11" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="AE10" s="11"/>
     </row>
@@ -4503,11 +5473,11 @@
       <c r="B11" s="6"/>
       <c r="C11" s="57"/>
       <c r="D11" s="57"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
       <c r="J11" s="57"/>
       <c r="K11" s="58"/>
       <c r="L11" s="6"/>
@@ -4532,13 +5502,13 @@
         <v>32</v>
       </c>
       <c r="AB11" s="25" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="AC11" s="11" t="s">
         <v>60</v>
       </c>
       <c r="AD11" s="11" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AE11" s="11"/>
     </row>
@@ -4547,11 +5517,11 @@
       <c r="B12" s="6"/>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
       <c r="J12" s="57"/>
       <c r="K12" s="57"/>
       <c r="L12" s="6"/>
@@ -4573,17 +5543,17 @@
         <v>52</v>
       </c>
       <c r="AA12" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB12" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC12" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AD12" s="11"/>
       <c r="AE12" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4591,11 +5561,11 @@
       <c r="B13" s="6"/>
       <c r="C13" s="57"/>
       <c r="D13" s="57"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
       <c r="J13" s="57"/>
       <c r="K13" s="57"/>
       <c r="L13" s="6"/>
@@ -4617,17 +5587,17 @@
         <v>53</v>
       </c>
       <c r="AA13" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB13" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC13" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AD13" s="11"/>
       <c r="AE13" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4661,17 +5631,17 @@
         <v>54</v>
       </c>
       <c r="AA14" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB14" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC14" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AD14" s="11"/>
       <c r="AE14" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4693,37 +5663,37 @@
         <v>55</v>
       </c>
       <c r="AA15" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB15" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC15" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AD15" s="11"/>
       <c r="AE15" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="96" t="str">
+      <c r="C16" s="74" t="str">
         <f>Y11</f>
         <v>in5</v>
       </c>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="97"/>
-      <c r="L16" s="97"/>
-      <c r="M16" s="97"/>
-      <c r="N16" s="97"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="75"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
@@ -4734,43 +5704,43 @@
       <c r="V16" s="7"/>
       <c r="W16" s="7"/>
       <c r="Y16" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Z16" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA16" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB16" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC16" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AD16" s="11"/>
       <c r="AE16" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="96" t="str">
+      <c r="C17" s="74" t="str">
         <f>Y10</f>
         <v>in4</v>
       </c>
-      <c r="D17" s="97"/>
-      <c r="E17" s="97"/>
-      <c r="F17" s="97"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="97"/>
-      <c r="K17" s="97"/>
-      <c r="L17" s="97"/>
-      <c r="M17" s="97"/>
-      <c r="N17" s="97"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="75"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="75"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
@@ -4781,23 +5751,23 @@
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
       <c r="Y17" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Z17" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AA17" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB17" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC17" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="AB17" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC17" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="AD17" s="11"/>
       <c r="AE17" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4825,23 +5795,23 @@
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
       <c r="Y18" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z18" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA18" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB18" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC18" s="11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="AD18" s="11"/>
       <c r="AE18" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4869,23 +5839,23 @@
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="Y19" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Z19" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA19" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB19" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC19" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="AB19" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC19" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="AD19" s="11"/>
       <c r="AE19" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4913,23 +5883,23 @@
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
       <c r="Y20" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z20" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AA20" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB20" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC20" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="AB20" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC20" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="AD20" s="11"/>
       <c r="AE20" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4957,23 +5927,23 @@
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="Y21" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Z21" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AA21" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB21" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC21" s="11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AD21" s="11"/>
       <c r="AE21" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5001,23 +5971,23 @@
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
       <c r="Y22" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Z22" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AA22" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB22" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC22" s="11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AD22" s="11"/>
       <c r="AE22" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5045,23 +6015,23 @@
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="Y23" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z23" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AA23" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB23" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC23" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AD23" s="11"/>
       <c r="AE23" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5089,21 +6059,21 @@
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="Y24" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AA24" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB24" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC24" s="11"/>
       <c r="AD24" s="11"/>
       <c r="AE24" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5131,21 +6101,21 @@
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="Y25" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z25" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AA25" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB25" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC25" s="11"/>
       <c r="AD25" s="11"/>
       <c r="AE25" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5173,21 +6143,21 @@
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="Y26" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z26" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="Z26" s="25" t="s">
-        <v>87</v>
-      </c>
       <c r="AA26" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB26" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC26" s="11"/>
       <c r="AD26" s="11"/>
       <c r="AE26" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5215,21 +6185,21 @@
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="Y27" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z27" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AA27" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB27" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AC27" s="11"/>
       <c r="AD27" s="11"/>
       <c r="AE27" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5406,7 +6376,7 @@
     </row>
     <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="71"/>
@@ -5840,6 +6810,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="C17:N17"/>
     <mergeCell ref="A35:T35"/>
     <mergeCell ref="A1:T1"/>
@@ -5856,24 +6844,6 @@
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="I10:I13"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <hyperlinks>
@@ -5905,7 +6875,7 @@
   <dimension ref="A1:AN52"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6076,7 +7046,7 @@
         <v>61</v>
       </c>
       <c r="AE4" s="29" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AN4" s="23"/>
     </row>
@@ -6105,16 +7075,16 @@
       <c r="V5" s="14"/>
       <c r="W5" s="14"/>
       <c r="Y5" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Z5" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA5" s="24" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB5" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AC5" s="11" t="s">
         <v>56</v>
@@ -6155,16 +7125,16 @@
       <c r="V6" s="14"/>
       <c r="W6" s="14"/>
       <c r="Y6" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Z6" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AA6" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB6" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
@@ -6209,7 +7179,7 @@
         <v>24</v>
       </c>
       <c r="AA7" s="28" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AB7" s="25"/>
       <c r="AC7" s="11"/>
@@ -6252,7 +7222,7 @@
         <v>26</v>
       </c>
       <c r="AA8" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB8" s="25"/>
       <c r="AC8" s="11"/>
@@ -6294,7 +7264,7 @@
         <v>27</v>
       </c>
       <c r="AA9" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="11"/>
@@ -6339,7 +7309,7 @@
         <v>28</v>
       </c>
       <c r="AA10" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="11"/>
@@ -6384,13 +7354,13 @@
         <v>32</v>
       </c>
       <c r="AB11" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC11" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AD11" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE11" s="11"/>
       <c r="AF11" s="23"/>
@@ -6435,13 +7405,13 @@
         <v>32</v>
       </c>
       <c r="AB12" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC12" s="11" t="s">
         <v>58</v>
       </c>
       <c r="AD12" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE12" s="11"/>
     </row>
@@ -6479,13 +7449,13 @@
         <v>32</v>
       </c>
       <c r="AB13" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC13" s="11" t="s">
         <v>59</v>
       </c>
       <c r="AD13" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE13" s="11"/>
     </row>
@@ -6526,13 +7496,13 @@
         <v>32</v>
       </c>
       <c r="AB14" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC14" s="11" t="s">
         <v>60</v>
       </c>
       <c r="AD14" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE14" s="11"/>
     </row>
@@ -6570,13 +7540,13 @@
         <v>32</v>
       </c>
       <c r="AB15" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC15" s="11" t="s">
         <v>60</v>
       </c>
       <c r="AD15" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE15" s="11"/>
     </row>
@@ -6992,7 +7962,7 @@
       <c r="D32" s="73"/>
       <c r="E32" s="20"/>
       <c r="F32" s="67" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G32" s="67"/>
       <c r="H32" s="67"/>
@@ -7062,7 +8032,7 @@
     </row>
     <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="71"/>
@@ -7537,8 +8507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7557,28 +8527,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
       <c r="U1" s="48"/>
       <c r="V1" s="48"/>
       <c r="W1" s="48"/>
@@ -7594,41 +8564,41 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="119" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="78" t="str">
+      <c r="B2" s="120"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="126" t="str">
         <f>Y12</f>
         <v>in6</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="74" t="s">
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="103" t="str">
+      <c r="I2" s="120"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="77" t="str">
         <f>Y17</f>
         <v>in11</v>
       </c>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="116" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="117"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="119" t="str">
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="92"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="103" t="str">
         <f>Y21</f>
         <v>in15</v>
       </c>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="121"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="105"/>
       <c r="U2" s="49"/>
       <c r="V2" s="49"/>
       <c r="W2" s="49"/>
@@ -7643,36 +8613,36 @@
       <c r="AC2" s="26"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="81" t="str">
+      <c r="B3" s="116"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="128" t="str">
         <f>Y13</f>
         <v>in7</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="87" t="s">
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="88"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="104" t="str">
+      <c r="I3" s="98"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="79" t="str">
         <f>Y18</f>
         <v>in12</v>
       </c>
-      <c r="L3" s="105"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="122"/>
-      <c r="R3" s="123"/>
-      <c r="S3" s="123"/>
-      <c r="T3" s="124"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="106"/>
+      <c r="R3" s="107"/>
+      <c r="S3" s="107"/>
+      <c r="T3" s="108"/>
       <c r="U3" s="49"/>
       <c r="V3" s="49"/>
       <c r="W3" s="49"/>
@@ -7687,36 +8657,36 @@
       <c r="AC3" s="8"/>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="81" t="str">
+      <c r="B4" s="116"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="128" t="str">
         <f>Y14</f>
         <v>in8</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="87" t="s">
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="88"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="125" t="str">
+      <c r="O4" s="98"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="109" t="str">
         <f>Y22</f>
         <v>in16</v>
       </c>
-      <c r="R4" s="126"/>
-      <c r="S4" s="126"/>
-      <c r="T4" s="127"/>
+      <c r="R4" s="110"/>
+      <c r="S4" s="110"/>
+      <c r="T4" s="111"/>
       <c r="U4" s="49"/>
       <c r="V4" s="49"/>
       <c r="W4" s="49"/>
@@ -7739,40 +8709,40 @@
         <v>61</v>
       </c>
       <c r="AE4" s="29" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="81" t="str">
+      <c r="B5" s="116"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="128" t="str">
         <f>Y15</f>
         <v>in9</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="93" t="s">
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="94"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="110" t="str">
+      <c r="I5" s="116"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="85" t="str">
         <f>Y19</f>
         <v>in13</v>
       </c>
-      <c r="L5" s="111"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="92"/>
-      <c r="Q5" s="122"/>
-      <c r="R5" s="123"/>
-      <c r="S5" s="123"/>
-      <c r="T5" s="124"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="107"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="108"/>
       <c r="U5" s="49"/>
       <c r="V5" s="49"/>
       <c r="W5" s="49"/>
@@ -7795,41 +8765,41 @@
       <c r="AE5" s="11"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="99" t="str">
+      <c r="B6" s="101"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="122" t="str">
         <f>Y16</f>
         <v>in10</v>
       </c>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="84" t="s">
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="113" t="str">
+      <c r="I6" s="101"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="88" t="str">
         <f>Y20</f>
         <v>in14</v>
       </c>
-      <c r="L6" s="114"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" s="85"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="128" t="str">
+      <c r="L6" s="89"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="101"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="112" t="str">
         <f>Y23</f>
         <v>in17</v>
       </c>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
-      <c r="T6" s="130"/>
+      <c r="R6" s="113"/>
+      <c r="S6" s="113"/>
+      <c r="T6" s="114"/>
       <c r="U6" s="50"/>
       <c r="V6" s="50"/>
       <c r="W6" s="50"/>
@@ -7850,9 +8820,9 @@
       <c r="AE6" s="11"/>
     </row>
     <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
+      <c r="A7" s="125"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -7970,19 +8940,19 @@
       <c r="B10" s="6"/>
       <c r="C10" s="57"/>
       <c r="D10" s="57"/>
-      <c r="E10" s="98" t="s">
+      <c r="E10" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="98" t="s">
+      <c r="F10" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="98" t="s">
+      <c r="G10" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="98" t="s">
+      <c r="H10" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="98" t="s">
+      <c r="I10" s="118" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="57"/>
@@ -8018,11 +8988,11 @@
       <c r="B11" s="6"/>
       <c r="C11" s="57"/>
       <c r="D11" s="57"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
       <c r="J11" s="57"/>
       <c r="K11" s="58"/>
       <c r="L11" s="6"/>
@@ -8053,7 +9023,7 @@
         <v>60</v>
       </c>
       <c r="AD11" s="11" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="AE11" s="11"/>
     </row>
@@ -8062,11 +9032,11 @@
       <c r="B12" s="6"/>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
       <c r="J12" s="57"/>
       <c r="K12" s="57"/>
       <c r="L12" s="6"/>
@@ -8088,7 +9058,7 @@
         <v>52</v>
       </c>
       <c r="AA12" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB12" s="25" t="s">
         <v>51</v>
@@ -8102,11 +9072,11 @@
       <c r="B13" s="6"/>
       <c r="C13" s="57"/>
       <c r="D13" s="57"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
       <c r="J13" s="57"/>
       <c r="K13" s="57"/>
       <c r="L13" s="6"/>
@@ -8128,7 +9098,7 @@
         <v>53</v>
       </c>
       <c r="AA13" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB13" s="25" t="s">
         <v>51</v>
@@ -8168,7 +9138,7 @@
         <v>54</v>
       </c>
       <c r="AA14" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB14" s="25" t="s">
         <v>51</v>
@@ -8196,7 +9166,7 @@
         <v>55</v>
       </c>
       <c r="AA15" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB15" s="25" t="s">
         <v>51</v>
@@ -8208,21 +9178,21 @@
     <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="96" t="str">
+      <c r="C16" s="74" t="str">
         <f>Y11</f>
         <v>in5</v>
       </c>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="97"/>
-      <c r="L16" s="97"/>
-      <c r="M16" s="97"/>
-      <c r="N16" s="97"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="75"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
@@ -8233,13 +9203,13 @@
       <c r="V16" s="7"/>
       <c r="W16" s="7"/>
       <c r="Y16" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Z16" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA16" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB16" s="25" t="s">
         <v>51</v>
@@ -8273,13 +9243,13 @@
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
       <c r="Y17" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Z17" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AA17" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB17" s="25" t="s">
         <v>51</v>
@@ -8313,13 +9283,13 @@
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
       <c r="Y18" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z18" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA18" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB18" s="25" t="s">
         <v>51</v>
@@ -8353,13 +9323,13 @@
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="Y19" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Z19" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA19" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB19" s="25" t="s">
         <v>51</v>
@@ -8393,13 +9363,13 @@
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
       <c r="Y20" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z20" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AA20" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB20" s="25" t="s">
         <v>51</v>
@@ -8433,13 +9403,13 @@
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="Y21" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Z21" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AA21" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB21" s="25" t="s">
         <v>51</v>
@@ -8473,13 +9443,13 @@
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
       <c r="Y22" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Z22" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AA22" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB22" s="25" t="s">
         <v>51</v>
@@ -8513,13 +9483,13 @@
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="Y23" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Z23" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AA23" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB23" s="25" t="s">
         <v>51</v>
@@ -8553,13 +9523,13 @@
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="Y24" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AA24" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB24" s="25" t="s">
         <v>51</v>
@@ -8593,13 +9563,13 @@
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="Y25" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z25" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AA25" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB25" s="25" t="s">
         <v>51</v>
@@ -8633,13 +9603,13 @@
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="Y26" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z26" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="Z26" s="25" t="s">
-        <v>87</v>
-      </c>
       <c r="AA26" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB26" s="25" t="s">
         <v>51</v>
@@ -8673,13 +9643,13 @@
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="Y27" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z27" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AA27" s="28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AB27" s="25" t="s">
         <v>51</v>
@@ -8862,7 +9832,7 @@
     </row>
     <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="71"/>
@@ -9296,14 +10266,16 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="A35:T35"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P3"/>
+    <mergeCell ref="Q2:T3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J4"/>
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="K3:M4"/>
     <mergeCell ref="A4:C4"/>
@@ -9319,16 +10291,14 @@
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="N6:P6"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P3"/>
-    <mergeCell ref="Q2:T3"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="A35:T35"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="I10:I13"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -9357,7 +10327,7 @@
   <dimension ref="A1:AN52"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+      <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9528,7 +10498,7 @@
         <v>61</v>
       </c>
       <c r="AE4" s="29" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AN4" s="23"/>
     </row>
@@ -9557,16 +10527,16 @@
       <c r="V5" s="14"/>
       <c r="W5" s="14"/>
       <c r="Y5" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Z5" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA5" s="24" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB5" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AC5" s="11" t="s">
         <v>56</v>
@@ -9607,16 +10577,16 @@
       <c r="V6" s="14"/>
       <c r="W6" s="14"/>
       <c r="Y6" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Z6" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AA6" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB6" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
@@ -9661,7 +10631,7 @@
         <v>24</v>
       </c>
       <c r="AA7" s="28" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AB7" s="25"/>
       <c r="AC7" s="11"/>
@@ -9704,7 +10674,7 @@
         <v>26</v>
       </c>
       <c r="AA8" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB8" s="25"/>
       <c r="AC8" s="11"/>
@@ -9746,7 +10716,7 @@
         <v>27</v>
       </c>
       <c r="AA9" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="11"/>
@@ -9791,7 +10761,7 @@
         <v>28</v>
       </c>
       <c r="AA10" s="28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="11"/>
@@ -9836,13 +10806,13 @@
         <v>32</v>
       </c>
       <c r="AB11" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC11" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AD11" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE11" s="11"/>
       <c r="AF11" s="23"/>
@@ -9887,13 +10857,13 @@
         <v>32</v>
       </c>
       <c r="AB12" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC12" s="11" t="s">
         <v>58</v>
       </c>
       <c r="AD12" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE12" s="11"/>
     </row>
@@ -9931,13 +10901,13 @@
         <v>32</v>
       </c>
       <c r="AB13" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC13" s="11" t="s">
         <v>59</v>
       </c>
       <c r="AD13" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE13" s="11"/>
     </row>
@@ -9978,13 +10948,13 @@
         <v>32</v>
       </c>
       <c r="AB14" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC14" s="11" t="s">
         <v>60</v>
       </c>
       <c r="AD14" s="11" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="AE14" s="11"/>
     </row>
@@ -10429,7 +11399,7 @@
       <c r="D32" s="73"/>
       <c r="E32" s="20"/>
       <c r="F32" s="67" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G32" s="67"/>
       <c r="H32" s="67"/>
@@ -10499,7 +11469,7 @@
     </row>
     <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="71"/>
@@ -10975,7 +11945,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11002,7 +11972,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="61" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
@@ -11037,6 +12007,1288 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="61"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.125" customWidth="1"/>
+    <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>255</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>259</v>
+      </c>
+      <c r="B22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>260</v>
+      </c>
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>261</v>
+      </c>
+      <c r="B24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>262</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>263</v>
+      </c>
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>264</v>
+      </c>
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>265</v>
+      </c>
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>267</v>
+      </c>
+      <c r="B30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>268</v>
+      </c>
+      <c r="B31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>269</v>
+      </c>
+      <c r="B32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>270</v>
+      </c>
+      <c r="B34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>271</v>
+      </c>
+      <c r="B35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>272</v>
+      </c>
+      <c r="B36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>273</v>
+      </c>
+      <c r="B37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>274</v>
+      </c>
+      <c r="B38" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>275</v>
+      </c>
+      <c r="B39" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>276</v>
+      </c>
+      <c r="B40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>277</v>
+      </c>
+      <c r="B41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>278</v>
+      </c>
+      <c r="B42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>279</v>
+      </c>
+      <c r="B43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>280</v>
+      </c>
+      <c r="B44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>281</v>
+      </c>
+      <c r="B45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>282</v>
+      </c>
+      <c r="B46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>283</v>
+      </c>
+      <c r="B47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>284</v>
+      </c>
+      <c r="B48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>285</v>
+      </c>
+      <c r="B49" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>287</v>
+      </c>
+      <c r="B50" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>289</v>
+      </c>
+      <c r="B51" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>291</v>
+      </c>
+      <c r="B52" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>293</v>
+      </c>
+      <c r="B53" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>295</v>
+      </c>
+      <c r="B54" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>297</v>
+      </c>
+      <c r="B55" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>299</v>
+      </c>
+      <c r="B56" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>301</v>
+      </c>
+      <c r="B57" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>303</v>
+      </c>
+      <c r="B58" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>305</v>
+      </c>
+      <c r="B59" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>307</v>
+      </c>
+      <c r="B60" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>309</v>
+      </c>
+      <c r="B61" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>311</v>
+      </c>
+      <c r="B62" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>313</v>
+      </c>
+      <c r="B63" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>315</v>
+      </c>
+      <c r="B64" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>317</v>
+      </c>
+      <c r="B65" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>319</v>
+      </c>
+      <c r="B66" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>321</v>
+      </c>
+      <c r="B67" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>323</v>
+      </c>
+      <c r="B69" t="s">
+        <v>148</v>
+      </c>
+      <c r="C69" t="s">
+        <v>149</v>
+      </c>
+      <c r="D69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>324</v>
+      </c>
+      <c r="B70" t="s">
+        <v>148</v>
+      </c>
+      <c r="C70" t="s">
+        <v>151</v>
+      </c>
+      <c r="D70" t="s">
+        <v>152</v>
+      </c>
+      <c r="E70" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>325</v>
+      </c>
+      <c r="B71" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>326</v>
+      </c>
+      <c r="B72" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" t="s">
+        <v>151</v>
+      </c>
+      <c r="D72" t="s">
+        <v>156</v>
+      </c>
+      <c r="E72" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>327</v>
+      </c>
+      <c r="B73" t="s">
+        <v>148</v>
+      </c>
+      <c r="C73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" t="s">
+        <v>157</v>
+      </c>
+      <c r="E73" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>328</v>
+      </c>
+      <c r="B74" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" t="s">
+        <v>159</v>
+      </c>
+      <c r="E74" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>329</v>
+      </c>
+      <c r="B76" t="s">
+        <v>113</v>
+      </c>
+      <c r="C76" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>330</v>
+      </c>
+      <c r="B77" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
+        <v>331</v>
+      </c>
+      <c r="B79" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
+        <v>332</v>
+      </c>
+      <c r="B80" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
+        <v>333</v>
+      </c>
+      <c r="B81" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>334</v>
+      </c>
+      <c r="B82" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A83" t="s">
+        <v>335</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>336</v>
+      </c>
+      <c r="B84" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A85" t="s">
+        <v>337</v>
+      </c>
+      <c r="B85" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>338</v>
+      </c>
+      <c r="B86" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A87" t="s">
+        <v>339</v>
+      </c>
+      <c r="B87" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>340</v>
+      </c>
+      <c r="B88" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A89" t="s">
+        <v>341</v>
+      </c>
+      <c r="B89" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A90" t="s">
+        <v>342</v>
+      </c>
+      <c r="B90" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A91" t="s">
+        <v>343</v>
+      </c>
+      <c r="B91" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
+        <v>344</v>
+      </c>
+      <c r="B92" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
+        <v>345</v>
+      </c>
+      <c r="B93" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A94" t="s">
+        <v>346</v>
+      </c>
+      <c r="B94" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A95" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A96" t="s">
+        <v>347</v>
+      </c>
+      <c r="B96" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>348</v>
+      </c>
+      <c r="B97" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A98" t="s">
+        <v>349</v>
+      </c>
+      <c r="B98" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>350</v>
+      </c>
+      <c r="B99" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A100" t="s">
+        <v>351</v>
+      </c>
+      <c r="B100" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A101" t="s">
+        <v>352</v>
+      </c>
+      <c r="B101" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A102" t="s">
+        <v>353</v>
+      </c>
+      <c r="B102" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A103" t="s">
+        <v>354</v>
+      </c>
+      <c r="B103" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A104" t="s">
+        <v>355</v>
+      </c>
+      <c r="B104" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A105" t="s">
+        <v>356</v>
+      </c>
+      <c r="B105" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A106" t="s">
+        <v>357</v>
+      </c>
+      <c r="B106" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A107" t="s">
+        <v>358</v>
+      </c>
+      <c r="B107" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A108" t="s">
+        <v>359</v>
+      </c>
+      <c r="B108" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A109" t="s">
+        <v>360</v>
+      </c>
+      <c r="B109" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A110" t="s">
+        <v>361</v>
+      </c>
+      <c r="B110" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A111" t="s">
+        <v>362</v>
+      </c>
+      <c r="B111" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A112" t="s">
+        <v>363</v>
+      </c>
+      <c r="B112" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A113" t="s">
+        <v>364</v>
+      </c>
+      <c r="B113" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A114" t="s">
+        <v>365</v>
+      </c>
+      <c r="B114" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A115" t="s">
+        <v>366</v>
+      </c>
+      <c r="B115" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A116" t="s">
+        <v>367</v>
+      </c>
+      <c r="B116" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A117" t="s">
+        <v>368</v>
+      </c>
+      <c r="B117" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A118" t="s">
+        <v>369</v>
+      </c>
+      <c r="B118" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A119" t="s">
+        <v>370</v>
+      </c>
+      <c r="B119" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A120" t="s">
+        <v>371</v>
+      </c>
+      <c r="B120" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A121" t="s">
+        <v>372</v>
+      </c>
+      <c r="B121" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A122" t="s">
+        <v>373</v>
+      </c>
+      <c r="B122" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A123" t="s">
+        <v>374</v>
+      </c>
+      <c r="B123" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A124" t="s">
+        <v>375</v>
+      </c>
+      <c r="B124" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A125" t="s">
+        <v>376</v>
+      </c>
+      <c r="B125" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A126" t="s">
+        <v>377</v>
+      </c>
+      <c r="B126" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A127" t="s">
+        <v>378</v>
+      </c>
+      <c r="B127" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A128" t="s">
+        <v>379</v>
+      </c>
+      <c r="B128" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A129" t="s">
+        <v>380</v>
+      </c>
+      <c r="B129" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A130" t="s">
+        <v>381</v>
+      </c>
+      <c r="B130" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A131" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A132" t="s">
+        <v>382</v>
+      </c>
+      <c r="B132" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A133" t="s">
+        <v>383</v>
+      </c>
+      <c r="B133" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A134" t="s">
+        <v>384</v>
+      </c>
+      <c r="B134" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A135" t="s">
+        <v>385</v>
+      </c>
+      <c r="B135" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A136" t="s">
+        <v>386</v>
+      </c>
+      <c r="B136" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A137" t="s">
+        <v>387</v>
+      </c>
+      <c r="B137" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A138" t="s">
+        <v>388</v>
+      </c>
+      <c r="B138" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A139" t="s">
+        <v>389</v>
+      </c>
+      <c r="B139" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A140" t="s">
+        <v>390</v>
+      </c>
+      <c r="B140" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A141" t="s">
+        <v>391</v>
+      </c>
+      <c r="B141" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A142" t="s">
+        <v>392</v>
+      </c>
+      <c r="B142" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A143" t="s">
+        <v>393</v>
+      </c>
+      <c r="B143" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A144" t="s">
+        <v>394</v>
+      </c>
+      <c r="B144" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A145" t="s">
+        <v>395</v>
+      </c>
+      <c r="B145" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A146" t="s">
+        <v>396</v>
+      </c>
+      <c r="B146" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A147" t="s">
+        <v>397</v>
+      </c>
+      <c r="B147" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A148" t="s">
+        <v>398</v>
+      </c>
+      <c r="B148" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A149" t="s">
+        <v>399</v>
+      </c>
+      <c r="B149" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A150" t="s">
+        <v>400</v>
+      </c>
+      <c r="B150" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A151" t="s">
+        <v>401</v>
+      </c>
+      <c r="B151" t="s">
+        <v>402</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
change html create logic
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="825" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="825"/>
   </bookViews>
   <sheets>
     <sheet name="home" sheetId="22" r:id="rId1"/>
@@ -43,8 +43,97 @@
             <family val="3"/>
             <charset val="128"/>
           </rPr>
-          <t xml:space="preserve">#628DB6
-</t>
+          <t>VLINE</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W16</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W13</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W13</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W13</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W13</t>
         </r>
       </text>
     </comment>
@@ -59,7 +148,7 @@
             <family val="3"/>
             <charset val="128"/>
           </rPr>
-          <t>#ffffdd;#aaa</t>
+          <t>CP</t>
         </r>
       </text>
     </comment>
@@ -73,208 +162,6 @@
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>#d7e4bc</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A35" authorId="0" shapeId="0">
       <text>
         <r>
@@ -286,7 +173,7 @@
             <family val="3"/>
             <charset val="128"/>
           </rPr>
-          <t>#ffffdd;#aaa</t>
+          <t>CP</t>
         </r>
       </text>
     </comment>
@@ -327,7 +214,7 @@
             <family val="3"/>
             <charset val="128"/>
           </rPr>
-          <t>#ffffdd;#aaa</t>
+          <t>CP</t>
         </r>
       </text>
     </comment>
@@ -554,7 +441,7 @@
             <family val="3"/>
             <charset val="128"/>
           </rPr>
-          <t>#ffffdd;#aaa</t>
+          <t>CP</t>
         </r>
       </text>
     </comment>
@@ -595,7 +482,7 @@
             <family val="3"/>
             <charset val="128"/>
           </rPr>
-          <t>#ffffdd;#aaa</t>
+          <t>CP</t>
         </r>
       </text>
     </comment>
@@ -604,7 +491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="480">
   <si>
     <t>action</t>
     <phoneticPr fontId="5"/>
@@ -1772,9 +1659,6 @@
     <t>.BR2</t>
   </si>
   <si>
-    <t>.BR3</t>
-  </si>
-  <si>
     <t>.BR4</t>
   </si>
   <si>
@@ -2002,6 +1886,214 @@
   </si>
   <si>
     <t>/*cell left*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>background-color:#628DB6;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.CP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>color:#aaa;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>font-size: 11px;</t>
+  </si>
+  <si>
+    <t>font-size: 11px;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*copyright*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/*font size*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.F1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.F2</t>
+  </si>
+  <si>
+    <t>.F3</t>
+  </si>
+  <si>
+    <t>.F4</t>
+  </si>
+  <si>
+    <t>.F5</t>
+  </si>
+  <si>
+    <t>.F6</t>
+  </si>
+  <si>
+    <t>.F7</t>
+  </si>
+  <si>
+    <t>.F8</t>
+  </si>
+  <si>
+    <t>.F9</t>
+  </si>
+  <si>
+    <t>.F10</t>
+  </si>
+  <si>
+    <t>.F11</t>
+  </si>
+  <si>
+    <t>.F12</t>
+  </si>
+  <si>
+    <t>.F13</t>
+  </si>
+  <si>
+    <t>.F14</t>
+  </si>
+  <si>
+    <t>.F15</t>
+  </si>
+  <si>
+    <t>.F16</t>
+  </si>
+  <si>
+    <t>.F17</t>
+  </si>
+  <si>
+    <t>.F18</t>
+  </si>
+  <si>
+    <t>.F19</t>
+  </si>
+  <si>
+    <t>.F20</t>
+  </si>
+  <si>
+    <t>.F21</t>
+  </si>
+  <si>
+    <t>.F22</t>
+  </si>
+  <si>
+    <t>.F23</t>
+  </si>
+  <si>
+    <t>.F24</t>
+  </si>
+  <si>
+    <t>.F25</t>
+  </si>
+  <si>
+    <t>font-size: 1px;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>font-size: 2px;</t>
+  </si>
+  <si>
+    <t>font-size: 3px;</t>
+  </si>
+  <si>
+    <t>font-size: 4px;</t>
+  </si>
+  <si>
+    <t>font-size: 5px;</t>
+  </si>
+  <si>
+    <t>font-size: 6px;</t>
+  </si>
+  <si>
+    <t>font-size: 7px;</t>
+  </si>
+  <si>
+    <t>font-size: 8px;</t>
+  </si>
+  <si>
+    <t>font-size: 9px;</t>
+  </si>
+  <si>
+    <t>font-size: 10px;</t>
+  </si>
+  <si>
+    <t>font-size: 12px;</t>
+  </si>
+  <si>
+    <t>font-size: 13px;</t>
+  </si>
+  <si>
+    <t>font-size: 14px;</t>
+  </si>
+  <si>
+    <t>font-size: 15px;</t>
+  </si>
+  <si>
+    <t>font-size: 16px;</t>
+  </si>
+  <si>
+    <t>font-size: 17px;</t>
+  </si>
+  <si>
+    <t>font-size: 18px;</t>
+  </si>
+  <si>
+    <t>font-size: 19px;</t>
+  </si>
+  <si>
+    <t>font-size: 20px;</t>
+  </si>
+  <si>
+    <t>font-size: 21px;</t>
+  </si>
+  <si>
+    <t>font-size: 22px;</t>
+  </si>
+  <si>
+    <t>font-size: 23px;</t>
+  </si>
+  <si>
+    <t>font-size: 24px;</t>
+  </si>
+  <si>
+    <t>font-size: 25px;</t>
+  </si>
+  <si>
+    <t>フリガナ</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>.CLBL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.VLINE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>background-color:#ffffdd;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.CINP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>background-color:#d7e4bc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>background-color:#d7e4bc;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>.BR3</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2308,7 +2400,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -2647,6 +2739,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2658,7 +2779,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2862,19 +2983,111 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2931,42 +3144,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="25" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3003,60 +3180,43 @@
     <xf numFmtId="0" fontId="27" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3368,8 +3528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AD15" sqref="AD15"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3728,26 +3888,26 @@
       <c r="AI8" s="23"/>
     </row>
     <row r="9" spans="1:40" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
       <c r="D9" s="73"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+      <c r="I9" s="133"/>
+      <c r="J9" s="133"/>
+      <c r="K9" s="133"/>
+      <c r="L9" s="133"/>
+      <c r="M9" s="133"/>
+      <c r="N9" s="133"/>
+      <c r="O9" s="133"/>
+      <c r="P9" s="133"/>
+      <c r="Q9" s="133"/>
+      <c r="R9" s="133"/>
+      <c r="S9" s="133"/>
+      <c r="T9" s="133"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -3776,22 +3936,19 @@
       <c r="D10" s="73"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="72" t="str">
-        <f>Y11</f>
-        <v>in5</v>
-      </c>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72"/>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="72"/>
-      <c r="R10" s="72"/>
-      <c r="S10" s="72"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="135"/>
+      <c r="J10" s="135"/>
+      <c r="K10" s="135"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="135"/>
+      <c r="N10" s="135"/>
+      <c r="O10" s="135"/>
+      <c r="P10" s="135"/>
+      <c r="Q10" s="135"/>
+      <c r="R10" s="135"/>
+      <c r="S10" s="136"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
@@ -3869,22 +4026,19 @@
       <c r="D12" s="73"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="72" t="str">
-        <f>Y12</f>
-        <v>in6</v>
-      </c>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
-      <c r="R12" s="72"/>
-      <c r="S12" s="72"/>
+      <c r="G12" s="137"/>
+      <c r="H12" s="137"/>
+      <c r="I12" s="137"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="137"/>
+      <c r="L12" s="137"/>
+      <c r="M12" s="137"/>
+      <c r="N12" s="137"/>
+      <c r="O12" s="137"/>
+      <c r="P12" s="137"/>
+      <c r="Q12" s="137"/>
+      <c r="R12" s="137"/>
+      <c r="S12" s="137"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
@@ -3960,22 +4114,19 @@
       <c r="D14" s="73"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="72" t="str">
-        <f>Y13</f>
-        <v>in7</v>
-      </c>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="72"/>
-      <c r="Q14" s="72"/>
-      <c r="R14" s="72"/>
-      <c r="S14" s="72"/>
+      <c r="G14" s="138"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
+      <c r="N14" s="138"/>
+      <c r="O14" s="138"/>
+      <c r="P14" s="138"/>
+      <c r="Q14" s="138"/>
+      <c r="R14" s="138"/>
+      <c r="S14" s="138"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
@@ -4007,19 +4158,19 @@
       <c r="D15" s="73"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="132"/>
+      <c r="I15" s="132"/>
+      <c r="J15" s="132"/>
+      <c r="K15" s="132"/>
+      <c r="L15" s="132"/>
+      <c r="M15" s="132"/>
+      <c r="N15" s="132"/>
+      <c r="O15" s="132"/>
+      <c r="P15" s="132"/>
+      <c r="Q15" s="132"/>
+      <c r="R15" s="132"/>
+      <c r="S15" s="140"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
@@ -4039,22 +4190,19 @@
       <c r="D16" s="73"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="72" t="str">
-        <f>Y14</f>
-        <v>in8</v>
-      </c>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="72"/>
+      <c r="G16" s="143"/>
+      <c r="H16" s="139"/>
+      <c r="I16" s="139"/>
+      <c r="J16" s="139"/>
+      <c r="K16" s="139"/>
+      <c r="L16" s="139"/>
+      <c r="M16" s="139"/>
+      <c r="N16" s="139"/>
+      <c r="O16" s="139"/>
+      <c r="P16" s="139"/>
+      <c r="Q16" s="139"/>
+      <c r="R16" s="139"/>
+      <c r="S16" s="141"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
@@ -4948,7 +5096,7 @@
     <protectedRange sqref="F6" name="タイトル1"/>
     <protectedRange sqref="F32" name="会社名"/>
   </protectedRanges>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="F6:S6"/>
     <mergeCell ref="F32:S32"/>
     <mergeCell ref="F7:M7"/>
@@ -4956,8 +5104,10 @@
     <mergeCell ref="G10:S10"/>
     <mergeCell ref="G12:S12"/>
     <mergeCell ref="G14:S14"/>
-    <mergeCell ref="G16:S16"/>
     <mergeCell ref="D1:D34"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:T9"/>
+    <mergeCell ref="G15:S16"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -4987,7 +5137,7 @@
   <dimension ref="A1:AE52"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AQ18" sqref="AQ18"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5006,28 +5156,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
+      <c r="Q1" s="102"/>
+      <c r="R1" s="102"/>
+      <c r="S1" s="102"/>
+      <c r="T1" s="102"/>
       <c r="U1" s="48"/>
       <c r="V1" s="48"/>
       <c r="W1" s="48"/>
@@ -5043,41 +5193,41 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="119" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="126" t="str">
+      <c r="A2" s="77" t="s">
+        <v>472</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="99" t="str">
         <f>Y12</f>
         <v>in6</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="119" t="s">
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="120"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="77" t="str">
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="103" t="str">
         <f>Y17</f>
         <v>in11</v>
       </c>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="91" t="s">
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="92"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="103" t="str">
+      <c r="O2" s="117"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="119" t="str">
         <f>Y21</f>
         <v>in15</v>
       </c>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="105"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="121"/>
       <c r="U2" s="49"/>
       <c r="V2" s="49"/>
       <c r="W2" s="49"/>
@@ -5092,36 +5242,36 @@
       <c r="AC2" s="26"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="128" t="str">
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="74" t="str">
         <f>Y13</f>
         <v>in7</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="97" t="s">
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="98"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="79" t="str">
+      <c r="I3" s="81"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="104" t="str">
         <f>Y18</f>
         <v>in12</v>
       </c>
-      <c r="L3" s="80"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="108"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="122"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
+      <c r="T3" s="124"/>
       <c r="U3" s="49"/>
       <c r="V3" s="49"/>
       <c r="W3" s="49"/>
@@ -5136,36 +5286,36 @@
       <c r="AC3" s="8"/>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="116"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="128" t="str">
+      <c r="B4" s="87"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="74" t="str">
         <f>Y14</f>
         <v>in8</v>
       </c>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="97" t="s">
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="98"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="109" t="str">
+      <c r="O4" s="81"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="125" t="str">
         <f>Y22</f>
         <v>in16</v>
       </c>
-      <c r="R4" s="110"/>
-      <c r="S4" s="110"/>
-      <c r="T4" s="111"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+      <c r="T4" s="127"/>
       <c r="U4" s="49"/>
       <c r="V4" s="49"/>
       <c r="W4" s="49"/>
@@ -5192,36 +5342,36 @@
       </c>
     </row>
     <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="116"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="128" t="str">
+      <c r="B5" s="87"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="74" t="str">
         <f>Y15</f>
         <v>in9</v>
       </c>
-      <c r="E5" s="129"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="115" t="s">
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="116"/>
-      <c r="J5" s="117"/>
-      <c r="K5" s="85" t="str">
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="110" t="str">
         <f>Y19</f>
         <v>in13</v>
       </c>
-      <c r="L5" s="86"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="94"/>
-      <c r="O5" s="95"/>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="108"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="123"/>
+      <c r="T5" s="124"/>
       <c r="U5" s="49"/>
       <c r="V5" s="49"/>
       <c r="W5" s="49"/>
@@ -5244,41 +5394,41 @@
       <c r="AE5" s="11"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="122" t="str">
+      <c r="B6" s="90"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="95" t="str">
         <f>Y16</f>
         <v>in10</v>
       </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="100" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="88" t="str">
+      <c r="I6" s="90"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="113" t="str">
         <f>Y20</f>
         <v>in14</v>
       </c>
-      <c r="L6" s="89"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="100" t="s">
+      <c r="L6" s="114"/>
+      <c r="M6" s="115"/>
+      <c r="N6" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="O6" s="101"/>
-      <c r="P6" s="102"/>
-      <c r="Q6" s="112" t="str">
+      <c r="O6" s="90"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="128" t="str">
         <f>Y23</f>
         <v>in17</v>
       </c>
-      <c r="R6" s="113"/>
-      <c r="S6" s="113"/>
-      <c r="T6" s="114"/>
+      <c r="R6" s="129"/>
+      <c r="S6" s="129"/>
+      <c r="T6" s="130"/>
       <c r="U6" s="50"/>
       <c r="V6" s="50"/>
       <c r="W6" s="50"/>
@@ -5299,9 +5449,9 @@
       <c r="AE6" s="11"/>
     </row>
     <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="125"/>
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
+      <c r="A7" s="98"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -5419,19 +5569,19 @@
       <c r="B10" s="6"/>
       <c r="C10" s="57"/>
       <c r="D10" s="57"/>
-      <c r="E10" s="118" t="s">
+      <c r="E10" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="118" t="s">
+      <c r="F10" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="118" t="s">
+      <c r="G10" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="118" t="s">
+      <c r="H10" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="118" t="s">
+      <c r="I10" s="94" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="57"/>
@@ -5473,11 +5623,11 @@
       <c r="B11" s="6"/>
       <c r="C11" s="57"/>
       <c r="D11" s="57"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
       <c r="J11" s="57"/>
       <c r="K11" s="58"/>
       <c r="L11" s="6"/>
@@ -5517,11 +5667,11 @@
       <c r="B12" s="6"/>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
       <c r="J12" s="57"/>
       <c r="K12" s="57"/>
       <c r="L12" s="6"/>
@@ -5561,11 +5711,11 @@
       <c r="B13" s="6"/>
       <c r="C13" s="57"/>
       <c r="D13" s="57"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
       <c r="J13" s="57"/>
       <c r="K13" s="57"/>
       <c r="L13" s="6"/>
@@ -5679,21 +5829,21 @@
     <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="74" t="str">
+      <c r="C16" s="92" t="str">
         <f>Y11</f>
         <v>in5</v>
       </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
@@ -5726,21 +5876,21 @@
     <row r="17" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="74" t="str">
+      <c r="C17" s="92" t="str">
         <f>Y10</f>
         <v>in4</v>
       </c>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="93"/>
+      <c r="N17" s="93"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
@@ -6810,24 +6960,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="C17:N17"/>
     <mergeCell ref="A35:T35"/>
     <mergeCell ref="A1:T1"/>
@@ -6844,6 +6976,24 @@
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="I10:I13"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <hyperlinks>
@@ -6874,8 +7024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AA22" sqref="AA22"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8032,7 +8182,7 @@
     </row>
     <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="71"/>
@@ -8507,8 +8657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Z21" sqref="Z21"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8527,28 +8677,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
+      <c r="Q1" s="102"/>
+      <c r="R1" s="102"/>
+      <c r="S1" s="102"/>
+      <c r="T1" s="102"/>
       <c r="U1" s="48"/>
       <c r="V1" s="48"/>
       <c r="W1" s="48"/>
@@ -8564,41 +8714,41 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="126" t="str">
+      <c r="B2" s="78"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="99" t="str">
         <f>Y12</f>
         <v>in6</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="119" t="s">
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="120"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="77" t="str">
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="103" t="str">
         <f>Y17</f>
         <v>in11</v>
       </c>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="91" t="s">
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="92"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="103" t="str">
+      <c r="O2" s="117"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="119" t="str">
         <f>Y21</f>
         <v>in15</v>
       </c>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="105"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="121"/>
       <c r="U2" s="49"/>
       <c r="V2" s="49"/>
       <c r="W2" s="49"/>
@@ -8613,36 +8763,36 @@
       <c r="AC2" s="26"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="128" t="str">
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="74" t="str">
         <f>Y13</f>
         <v>in7</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="97" t="s">
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="98"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="79" t="str">
+      <c r="I3" s="81"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="104" t="str">
         <f>Y18</f>
         <v>in12</v>
       </c>
-      <c r="L3" s="80"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="108"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="122"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
+      <c r="T3" s="124"/>
       <c r="U3" s="49"/>
       <c r="V3" s="49"/>
       <c r="W3" s="49"/>
@@ -8657,36 +8807,36 @@
       <c r="AC3" s="8"/>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="116"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="128" t="str">
+      <c r="B4" s="87"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="74" t="str">
         <f>Y14</f>
         <v>in8</v>
       </c>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="97" t="s">
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="98"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="109" t="str">
+      <c r="O4" s="81"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="125" t="str">
         <f>Y22</f>
         <v>in16</v>
       </c>
-      <c r="R4" s="110"/>
-      <c r="S4" s="110"/>
-      <c r="T4" s="111"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+      <c r="T4" s="127"/>
       <c r="U4" s="49"/>
       <c r="V4" s="49"/>
       <c r="W4" s="49"/>
@@ -8713,36 +8863,36 @@
       </c>
     </row>
     <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="116"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="128" t="str">
+      <c r="B5" s="87"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="74" t="str">
         <f>Y15</f>
         <v>in9</v>
       </c>
-      <c r="E5" s="129"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="115" t="s">
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="116"/>
-      <c r="J5" s="117"/>
-      <c r="K5" s="85" t="str">
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="110" t="str">
         <f>Y19</f>
         <v>in13</v>
       </c>
-      <c r="L5" s="86"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="94"/>
-      <c r="O5" s="95"/>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="108"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="123"/>
+      <c r="T5" s="124"/>
       <c r="U5" s="49"/>
       <c r="V5" s="49"/>
       <c r="W5" s="49"/>
@@ -8765,41 +8915,41 @@
       <c r="AE5" s="11"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="122" t="str">
+      <c r="B6" s="90"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="95" t="str">
         <f>Y16</f>
         <v>in10</v>
       </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="100" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="88" t="str">
+      <c r="I6" s="90"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="113" t="str">
         <f>Y20</f>
         <v>in14</v>
       </c>
-      <c r="L6" s="89"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="100" t="s">
+      <c r="L6" s="114"/>
+      <c r="M6" s="115"/>
+      <c r="N6" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="O6" s="101"/>
-      <c r="P6" s="102"/>
-      <c r="Q6" s="112" t="str">
+      <c r="O6" s="90"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="128" t="str">
         <f>Y23</f>
         <v>in17</v>
       </c>
-      <c r="R6" s="113"/>
-      <c r="S6" s="113"/>
-      <c r="T6" s="114"/>
+      <c r="R6" s="129"/>
+      <c r="S6" s="129"/>
+      <c r="T6" s="130"/>
       <c r="U6" s="50"/>
       <c r="V6" s="50"/>
       <c r="W6" s="50"/>
@@ -8820,9 +8970,9 @@
       <c r="AE6" s="11"/>
     </row>
     <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="125"/>
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
+      <c r="A7" s="98"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -8940,19 +9090,19 @@
       <c r="B10" s="6"/>
       <c r="C10" s="57"/>
       <c r="D10" s="57"/>
-      <c r="E10" s="118" t="s">
+      <c r="E10" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="118" t="s">
+      <c r="F10" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="118" t="s">
+      <c r="G10" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="118" t="s">
+      <c r="H10" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="118" t="s">
+      <c r="I10" s="94" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="57"/>
@@ -8988,11 +9138,11 @@
       <c r="B11" s="6"/>
       <c r="C11" s="57"/>
       <c r="D11" s="57"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
       <c r="J11" s="57"/>
       <c r="K11" s="58"/>
       <c r="L11" s="6"/>
@@ -9032,11 +9182,11 @@
       <c r="B12" s="6"/>
       <c r="C12" s="57"/>
       <c r="D12" s="57"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
       <c r="J12" s="57"/>
       <c r="K12" s="57"/>
       <c r="L12" s="6"/>
@@ -9072,11 +9222,11 @@
       <c r="B13" s="6"/>
       <c r="C13" s="57"/>
       <c r="D13" s="57"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
       <c r="J13" s="57"/>
       <c r="K13" s="57"/>
       <c r="L13" s="6"/>
@@ -9178,21 +9328,21 @@
     <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="74" t="str">
+      <c r="C16" s="92" t="str">
         <f>Y11</f>
         <v>in5</v>
       </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
@@ -10266,16 +10416,14 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P3"/>
-    <mergeCell ref="Q2:T3"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="A35:T35"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="I10:I13"/>
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="K3:M4"/>
     <mergeCell ref="A4:C4"/>
@@ -10291,14 +10439,16 @@
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="N6:P6"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="A35:T35"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P3"/>
+    <mergeCell ref="Q2:T3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -10326,8 +10476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Z24" sqref="Z24"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11469,7 +11619,7 @@
     </row>
     <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="71"/>
@@ -11945,7 +12095,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12016,10 +12166,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12038,7 +12188,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -12115,7 +12265,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -12147,7 +12297,7 @@
         <v>250</v>
       </c>
       <c r="B13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -12304,7 +12454,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
@@ -12344,7 +12494,7 @@
         <v>274</v>
       </c>
       <c r="B38" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
@@ -12581,7 +12731,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
@@ -12646,7 +12796,7 @@
         <v>156</v>
       </c>
       <c r="E72" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
@@ -12685,7 +12835,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
@@ -12704,12 +12854,12 @@
         <v>330</v>
       </c>
       <c r="B77" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
@@ -12717,7 +12867,7 @@
         <v>331</v>
       </c>
       <c r="B79" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
@@ -12826,7 +12976,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>345</v>
+        <v>479</v>
       </c>
       <c r="B93" t="s">
         <v>175</v>
@@ -12834,7 +12984,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B94" t="s">
         <v>176</v>
@@ -12842,12 +12992,12 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B96" t="s">
         <v>177</v>
@@ -12855,7 +13005,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B97" t="s">
         <v>178</v>
@@ -12863,15 +13013,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B98" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B99" t="s">
         <v>179</v>
@@ -12879,7 +13029,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B100" t="s">
         <v>180</v>
@@ -12887,7 +13037,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B101" t="s">
         <v>181</v>
@@ -12895,7 +13045,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B102" t="s">
         <v>182</v>
@@ -12903,7 +13053,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B103" t="s">
         <v>183</v>
@@ -12911,7 +13061,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B104" t="s">
         <v>184</v>
@@ -12919,7 +13069,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B105" t="s">
         <v>185</v>
@@ -12927,7 +13077,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B106" t="s">
         <v>186</v>
@@ -12935,7 +13085,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B107" t="s">
         <v>187</v>
@@ -12943,7 +13093,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B108" t="s">
         <v>188</v>
@@ -12951,7 +13101,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B109" t="s">
         <v>189</v>
@@ -12959,7 +13109,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B110" t="s">
         <v>190</v>
@@ -12967,7 +13117,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B111" t="s">
         <v>191</v>
@@ -12975,7 +13125,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B112" t="s">
         <v>192</v>
@@ -12983,7 +13133,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B113" t="s">
         <v>193</v>
@@ -12991,7 +13141,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B114" t="s">
         <v>194</v>
@@ -12999,7 +13149,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B115" t="s">
         <v>195</v>
@@ -13007,7 +13157,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B116" t="s">
         <v>196</v>
@@ -13015,7 +13165,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B117" t="s">
         <v>197</v>
@@ -13023,7 +13173,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B118" t="s">
         <v>198</v>
@@ -13031,7 +13181,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B119" t="s">
         <v>199</v>
@@ -13039,7 +13189,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B120" t="s">
         <v>200</v>
@@ -13047,7 +13197,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B121" t="s">
         <v>201</v>
@@ -13055,7 +13205,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B122" t="s">
         <v>202</v>
@@ -13063,7 +13213,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B123" t="s">
         <v>203</v>
@@ -13071,7 +13221,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B124" t="s">
         <v>204</v>
@@ -13079,7 +13229,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B125" t="s">
         <v>205</v>
@@ -13087,7 +13237,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B126" t="s">
         <v>206</v>
@@ -13095,7 +13245,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B127" t="s">
         <v>207</v>
@@ -13103,7 +13253,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B128" t="s">
         <v>208</v>
@@ -13111,7 +13261,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B129" t="s">
         <v>209</v>
@@ -13119,7 +13269,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B130" t="s">
         <v>210</v>
@@ -13127,12 +13277,12 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B132" t="s">
         <v>211</v>
@@ -13140,7 +13290,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B133" t="s">
         <v>212</v>
@@ -13148,7 +13298,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B134" t="s">
         <v>213</v>
@@ -13156,7 +13306,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B135" t="s">
         <v>214</v>
@@ -13164,7 +13314,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B136" t="s">
         <v>215</v>
@@ -13172,7 +13322,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B137" t="s">
         <v>216</v>
@@ -13180,7 +13330,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B138" t="s">
         <v>217</v>
@@ -13188,7 +13338,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B139" t="s">
         <v>218</v>
@@ -13196,7 +13346,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B140" t="s">
         <v>219</v>
@@ -13204,7 +13354,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B141" t="s">
         <v>220</v>
@@ -13212,7 +13362,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B142" t="s">
         <v>221</v>
@@ -13220,7 +13370,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B143" t="s">
         <v>222</v>
@@ -13228,7 +13378,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B144" t="s">
         <v>223</v>
@@ -13236,7 +13386,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B145" t="s">
         <v>224</v>
@@ -13244,7 +13394,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B146" t="s">
         <v>225</v>
@@ -13252,7 +13402,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B147" t="s">
         <v>226</v>
@@ -13260,7 +13410,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B148" t="s">
         <v>227</v>
@@ -13268,7 +13418,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B149" t="s">
         <v>228</v>
@@ -13276,7 +13426,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A150" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B150" t="s">
         <v>229</v>
@@ -13284,14 +13434,263 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A151" t="s">
+        <v>400</v>
+      </c>
+      <c r="B151" t="s">
         <v>401</v>
       </c>
-      <c r="B151" t="s">
-        <v>402</v>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A152" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A153" t="s">
+        <v>423</v>
+      </c>
+      <c r="B153" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A154" t="s">
+        <v>424</v>
+      </c>
+      <c r="B154" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A155" t="s">
+        <v>425</v>
+      </c>
+      <c r="B155" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A156" t="s">
+        <v>426</v>
+      </c>
+      <c r="B156" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A157" t="s">
+        <v>427</v>
+      </c>
+      <c r="B157" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A158" t="s">
+        <v>428</v>
+      </c>
+      <c r="B158" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A159" t="s">
+        <v>429</v>
+      </c>
+      <c r="B159" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A160" t="s">
+        <v>430</v>
+      </c>
+      <c r="B160" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A161" t="s">
+        <v>431</v>
+      </c>
+      <c r="B161" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A162" t="s">
+        <v>432</v>
+      </c>
+      <c r="B162" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A163" t="s">
+        <v>433</v>
+      </c>
+      <c r="B163" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A164" t="s">
+        <v>434</v>
+      </c>
+      <c r="B164" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A165" t="s">
+        <v>435</v>
+      </c>
+      <c r="B165" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A166" t="s">
+        <v>436</v>
+      </c>
+      <c r="B166" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A167" t="s">
+        <v>437</v>
+      </c>
+      <c r="B167" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A168" t="s">
+        <v>438</v>
+      </c>
+      <c r="B168" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A169" t="s">
+        <v>439</v>
+      </c>
+      <c r="B169" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A170" t="s">
+        <v>440</v>
+      </c>
+      <c r="B170" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A171" t="s">
+        <v>441</v>
+      </c>
+      <c r="B171" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A172" t="s">
+        <v>442</v>
+      </c>
+      <c r="B172" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A173" t="s">
+        <v>443</v>
+      </c>
+      <c r="B173" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A174" t="s">
+        <v>444</v>
+      </c>
+      <c r="B174" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A175" t="s">
+        <v>445</v>
+      </c>
+      <c r="B175" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A176" t="s">
+        <v>446</v>
+      </c>
+      <c r="B176" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A177" t="s">
+        <v>447</v>
+      </c>
+      <c r="B177" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A178" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A179" t="s">
+        <v>417</v>
+      </c>
+      <c r="B179" t="s">
+        <v>475</v>
+      </c>
+      <c r="C179" t="s">
+        <v>418</v>
+      </c>
+      <c r="D179" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A180" t="s">
+        <v>473</v>
+      </c>
+      <c r="B180" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A181" t="s">
+        <v>474</v>
+      </c>
+      <c r="B181" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A182" t="s">
+        <v>476</v>
+      </c>
+      <c r="B182" t="s">
+        <v>477</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add file change watch
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -440,7 +440,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="505">
   <si>
     <t>action</t>
     <phoneticPr fontId="5"/>
@@ -2130,6 +2130,22 @@
   </si>
   <si>
     <t>loop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hahahahaha</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6856,7 +6872,7 @@
   <dimension ref="A1:AN52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7614,7 +7630,9 @@
       <c r="A20" s="156"/>
       <c r="B20" s="151"/>
       <c r="C20" s="151"/>
-      <c r="D20" s="157"/>
+      <c r="D20" s="157" t="s">
+        <v>502</v>
+      </c>
       <c r="E20" s="151"/>
       <c r="F20" s="151"/>
       <c r="G20" s="160"/>
@@ -7639,7 +7657,9 @@
       <c r="A21" s="156"/>
       <c r="B21" s="151"/>
       <c r="C21" s="151"/>
-      <c r="D21" s="157"/>
+      <c r="D21" s="157" t="s">
+        <v>503</v>
+      </c>
       <c r="E21" s="151"/>
       <c r="F21" s="151"/>
       <c r="G21" s="160"/>
@@ -7664,7 +7684,9 @@
       <c r="A22" s="156"/>
       <c r="B22" s="151"/>
       <c r="C22" s="151"/>
-      <c r="D22" s="157"/>
+      <c r="D22" s="157" t="s">
+        <v>501</v>
+      </c>
       <c r="E22" s="151"/>
       <c r="F22" s="151"/>
       <c r="G22" s="160"/>
@@ -7689,7 +7711,9 @@
       <c r="A23" s="156"/>
       <c r="B23" s="151"/>
       <c r="C23" s="151"/>
-      <c r="D23" s="157"/>
+      <c r="D23" s="157" t="s">
+        <v>501</v>
+      </c>
       <c r="E23" s="151"/>
       <c r="F23" s="151"/>
       <c r="G23" s="160"/>
@@ -7714,7 +7738,9 @@
       <c r="A24" s="156"/>
       <c r="B24" s="151"/>
       <c r="C24" s="151"/>
-      <c r="D24" s="157"/>
+      <c r="D24" s="157" t="s">
+        <v>503</v>
+      </c>
       <c r="E24" s="151"/>
       <c r="F24" s="151"/>
       <c r="G24" s="160"/>
@@ -7739,7 +7765,9 @@
       <c r="A25" s="156"/>
       <c r="B25" s="151"/>
       <c r="C25" s="151"/>
-      <c r="D25" s="157"/>
+      <c r="D25" s="157" t="s">
+        <v>503</v>
+      </c>
       <c r="E25" s="151"/>
       <c r="F25" s="151"/>
       <c r="G25" s="160"/>
@@ -7764,7 +7792,9 @@
       <c r="A26" s="156"/>
       <c r="B26" s="151"/>
       <c r="C26" s="151"/>
-      <c r="D26" s="157"/>
+      <c r="D26" s="157" t="s">
+        <v>504</v>
+      </c>
       <c r="E26" s="151"/>
       <c r="F26" s="151"/>
       <c r="G26" s="160"/>

</xml_diff>

<commit_message>
change js to outside
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="825" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="825"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="29" r:id="rId1"/>
@@ -82,6 +82,51 @@
             <charset val="128"/>
           </rPr>
           <t>W16</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W4 H2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W4 H2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>W5 H2</t>
         </r>
       </text>
     </comment>
@@ -2735,7 +2780,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3013,42 +3058,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -3060,6 +3069,19 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3079,45 +3101,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3174,6 +3164,30 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="23" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3209,6 +3223,70 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3519,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:S20"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26:S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4362,19 +4440,19 @@
       <c r="D23" s="92"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="61"/>
-      <c r="R23" s="61"/>
-      <c r="S23" s="61"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="157"/>
+      <c r="J23" s="158"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="157"/>
+      <c r="M23" s="157"/>
+      <c r="N23" s="158"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="157"/>
+      <c r="Q23" s="157"/>
+      <c r="R23" s="157"/>
+      <c r="S23" s="158"/>
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
@@ -4387,19 +4465,19 @@
       <c r="D24" s="92"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="61"/>
-      <c r="S24" s="61"/>
+      <c r="G24" s="159"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="160"/>
+      <c r="J24" s="161"/>
+      <c r="K24" s="159"/>
+      <c r="L24" s="160"/>
+      <c r="M24" s="160"/>
+      <c r="N24" s="161"/>
+      <c r="O24" s="159"/>
+      <c r="P24" s="160"/>
+      <c r="Q24" s="160"/>
+      <c r="R24" s="160"/>
+      <c r="S24" s="161"/>
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
       <c r="V24" s="7"/>
@@ -4437,19 +4515,19 @@
       <c r="D26" s="92"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
-      <c r="P26" s="61"/>
-      <c r="Q26" s="61"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="61"/>
+      <c r="G26" s="162"/>
+      <c r="H26" s="163"/>
+      <c r="I26" s="163"/>
+      <c r="J26" s="164"/>
+      <c r="K26" s="162"/>
+      <c r="L26" s="163"/>
+      <c r="M26" s="163"/>
+      <c r="N26" s="164"/>
+      <c r="O26" s="162"/>
+      <c r="P26" s="163"/>
+      <c r="Q26" s="163"/>
+      <c r="R26" s="163"/>
+      <c r="S26" s="164"/>
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
       <c r="V26" s="7"/>
@@ -4462,19 +4540,19 @@
       <c r="D27" s="92"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61"/>
+      <c r="G27" s="165"/>
+      <c r="H27" s="166"/>
+      <c r="I27" s="166"/>
+      <c r="J27" s="167"/>
+      <c r="K27" s="165"/>
+      <c r="L27" s="166"/>
+      <c r="M27" s="166"/>
+      <c r="N27" s="167"/>
+      <c r="O27" s="165"/>
+      <c r="P27" s="166"/>
+      <c r="Q27" s="166"/>
+      <c r="R27" s="166"/>
+      <c r="S27" s="167"/>
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
       <c r="V27" s="7"/>
@@ -5093,7 +5171,7 @@
     <protectedRange sqref="F6" name="タイトル1"/>
     <protectedRange sqref="F32" name="会社名"/>
   </protectedRanges>
-  <mergeCells count="10">
+  <mergeCells count="13">
     <mergeCell ref="A35:T35"/>
     <mergeCell ref="G14:S16"/>
     <mergeCell ref="G10:S12"/>
@@ -5104,6 +5182,9 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="E9:T9"/>
     <mergeCell ref="F32:S32"/>
+    <mergeCell ref="G23:J24"/>
+    <mergeCell ref="K23:N24"/>
+    <mergeCell ref="O23:S24"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -11476,8 +11557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -13116,28 +13197,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
-      <c r="P1" s="128"/>
-      <c r="Q1" s="128"/>
-      <c r="R1" s="128"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="128"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
       <c r="U1" s="45"/>
       <c r="V1" s="45"/>
       <c r="W1" s="45"/>
@@ -13153,41 +13234,41 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="148" t="s">
         <v>468</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="125" t="str">
+      <c r="B2" s="149"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="155" t="str">
         <f>Y12</f>
         <v>in6</v>
       </c>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="100" t="s">
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="148" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="101"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="129" t="str">
+      <c r="I2" s="149"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="113" t="str">
         <f>Y17</f>
         <v>in11</v>
       </c>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="142" t="s">
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="143"/>
-      <c r="P2" s="144"/>
-      <c r="Q2" s="145" t="str">
+      <c r="O2" s="128"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="136" t="str">
         <f>Y21</f>
         <v>in15</v>
       </c>
-      <c r="R2" s="146"/>
-      <c r="S2" s="146"/>
-      <c r="T2" s="147"/>
+      <c r="R2" s="137"/>
+      <c r="S2" s="137"/>
+      <c r="T2" s="138"/>
       <c r="U2" s="46"/>
       <c r="V2" s="46"/>
       <c r="W2" s="46"/>
@@ -13202,36 +13283,36 @@
       <c r="AC2" s="24"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="121" t="str">
+      <c r="B3" s="101"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="104" t="str">
         <f>Y13</f>
         <v>in7</v>
       </c>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="103" t="s">
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="104"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="130" t="str">
+      <c r="I3" s="134"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="115" t="str">
         <f>Y18</f>
         <v>in12</v>
       </c>
-      <c r="L3" s="131"/>
-      <c r="M3" s="132"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="148"/>
-      <c r="R3" s="149"/>
-      <c r="S3" s="149"/>
-      <c r="T3" s="150"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="132"/>
+      <c r="Q3" s="139"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140"/>
+      <c r="T3" s="141"/>
       <c r="U3" s="46"/>
       <c r="V3" s="46"/>
       <c r="W3" s="46"/>
@@ -13246,36 +13327,36 @@
       <c r="AC3" s="8"/>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="110"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="121" t="str">
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="104" t="str">
         <f>Y14</f>
         <v>in8</v>
       </c>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="103" t="s">
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="132"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="104"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="151" t="str">
+      <c r="O4" s="134"/>
+      <c r="P4" s="135"/>
+      <c r="Q4" s="142" t="str">
         <f>Y22</f>
         <v>in16</v>
       </c>
-      <c r="R4" s="152"/>
-      <c r="S4" s="152"/>
-      <c r="T4" s="153"/>
+      <c r="R4" s="143"/>
+      <c r="S4" s="143"/>
+      <c r="T4" s="144"/>
       <c r="U4" s="46"/>
       <c r="V4" s="46"/>
       <c r="W4" s="46"/>
@@ -13302,36 +13383,36 @@
       </c>
     </row>
     <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="121" t="str">
+      <c r="B5" s="101"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="104" t="str">
         <f>Y15</f>
         <v>in9</v>
       </c>
-      <c r="E5" s="122"/>
-      <c r="F5" s="122"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="109" t="s">
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="110"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="136" t="str">
+      <c r="I5" s="101"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="121" t="str">
         <f>Y19</f>
         <v>in13</v>
       </c>
-      <c r="L5" s="137"/>
-      <c r="M5" s="138"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="107"/>
-      <c r="P5" s="108"/>
-      <c r="Q5" s="148"/>
-      <c r="R5" s="149"/>
-      <c r="S5" s="149"/>
-      <c r="T5" s="150"/>
+      <c r="L5" s="122"/>
+      <c r="M5" s="123"/>
+      <c r="N5" s="130"/>
+      <c r="O5" s="131"/>
+      <c r="P5" s="132"/>
+      <c r="Q5" s="139"/>
+      <c r="R5" s="140"/>
+      <c r="S5" s="140"/>
+      <c r="T5" s="141"/>
       <c r="U5" s="46"/>
       <c r="V5" s="46"/>
       <c r="W5" s="46"/>
@@ -13354,41 +13435,41 @@
       <c r="AE5" s="10"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="114"/>
-      <c r="D6" s="118" t="str">
+      <c r="B6" s="108"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="151" t="str">
         <f>Y16</f>
         <v>in10</v>
       </c>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="112" t="s">
+      <c r="E6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="113"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="139" t="str">
+      <c r="I6" s="108"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="124" t="str">
         <f>Y20</f>
         <v>in14</v>
       </c>
-      <c r="L6" s="140"/>
-      <c r="M6" s="141"/>
-      <c r="N6" s="112" t="s">
+      <c r="L6" s="125"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="O6" s="113"/>
-      <c r="P6" s="114"/>
-      <c r="Q6" s="154" t="str">
+      <c r="O6" s="108"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="145" t="str">
         <f>Y23</f>
         <v>in17</v>
       </c>
-      <c r="R6" s="155"/>
-      <c r="S6" s="155"/>
-      <c r="T6" s="156"/>
+      <c r="R6" s="146"/>
+      <c r="S6" s="146"/>
+      <c r="T6" s="147"/>
       <c r="U6" s="47"/>
       <c r="V6" s="47"/>
       <c r="W6" s="47"/>
@@ -13409,9 +13490,9 @@
       <c r="AE6" s="10"/>
     </row>
     <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="124"/>
-      <c r="B7" s="124"/>
-      <c r="C7" s="124"/>
+      <c r="A7" s="154"/>
+      <c r="B7" s="154"/>
+      <c r="C7" s="154"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -13529,19 +13610,19 @@
       <c r="B10" s="6"/>
       <c r="C10" s="54"/>
       <c r="D10" s="54"/>
-      <c r="E10" s="117" t="s">
+      <c r="E10" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="117" t="s">
+      <c r="F10" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="117" t="s">
+      <c r="H10" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="117" t="s">
+      <c r="I10" s="103" t="s">
         <v>40</v>
       </c>
       <c r="J10" s="54"/>
@@ -13583,11 +13664,11 @@
       <c r="B11" s="6"/>
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="117"/>
-      <c r="H11" s="117"/>
-      <c r="I11" s="117"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
       <c r="J11" s="54"/>
       <c r="K11" s="55"/>
       <c r="L11" s="6"/>
@@ -13627,11 +13708,11 @@
       <c r="B12" s="6"/>
       <c r="C12" s="54"/>
       <c r="D12" s="54"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="117"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
       <c r="J12" s="54"/>
       <c r="K12" s="54"/>
       <c r="L12" s="6"/>
@@ -13671,11 +13752,11 @@
       <c r="B13" s="6"/>
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="117"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
       <c r="J13" s="54"/>
       <c r="K13" s="54"/>
       <c r="L13" s="6"/>
@@ -13789,21 +13870,21 @@
     <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="115" t="str">
+      <c r="C16" s="110" t="str">
         <f>Y11</f>
         <v>in5</v>
       </c>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="116"/>
-      <c r="K16" s="116"/>
-      <c r="L16" s="116"/>
-      <c r="M16" s="116"/>
-      <c r="N16" s="116"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="111"/>
+      <c r="I16" s="111"/>
+      <c r="J16" s="111"/>
+      <c r="K16" s="111"/>
+      <c r="L16" s="111"/>
+      <c r="M16" s="111"/>
+      <c r="N16" s="111"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
@@ -13836,21 +13917,21 @@
     <row r="17" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="115" t="str">
+      <c r="C17" s="110" t="str">
         <f>Y10</f>
         <v>in4</v>
       </c>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="116"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="116"/>
-      <c r="N17" s="116"/>
+      <c r="D17" s="111"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="111"/>
+      <c r="K17" s="111"/>
+      <c r="L17" s="111"/>
+      <c r="M17" s="111"/>
+      <c r="N17" s="111"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
@@ -14920,11 +15001,9 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D2:G2"/>
     <mergeCell ref="A35:T35"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="K2:M2"/>
@@ -14941,6 +15020,11 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="H3:J4"/>
     <mergeCell ref="H5:J5"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="C17:N17"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="C16:N16"/>
     <mergeCell ref="A3:C3"/>
@@ -14951,9 +15035,6 @@
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D5:G5"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D2:G2"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <hyperlinks>

</xml_diff>